<commit_message>
More data from today's drops
</commit_message>
<xml_diff>
--- a/Drops.xlsx
+++ b/Drops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="64">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t xml:space="preserve">2020/3/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/3/20</t>
   </si>
 </sst>
 </file>
@@ -485,8 +488,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ393"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B97" activeCellId="0" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4664,14 +4667,22 @@
       <c r="BI56" s="11"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
+      <c r="A57" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
+      <c r="H57" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
@@ -4727,9 +4738,15 @@
       <c r="BI57" s="12"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
+      <c r="A58" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
@@ -4749,7 +4766,9 @@
       <c r="T58" s="11"/>
       <c r="U58" s="11"/>
       <c r="V58" s="11"/>
-      <c r="W58" s="11"/>
+      <c r="W58" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X58" s="11"/>
       <c r="Y58" s="11"/>
       <c r="Z58" s="11"/>
@@ -4780,7 +4799,9 @@
       <c r="AY58" s="11"/>
       <c r="AZ58" s="11"/>
       <c r="BA58" s="11"/>
-      <c r="BB58" s="11"/>
+      <c r="BB58" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="BC58" s="11"/>
       <c r="BD58" s="11"/>
       <c r="BE58" s="11"/>
@@ -4790,9 +4811,15 @@
       <c r="BI58" s="11"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
+      <c r="A59" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
@@ -4823,7 +4850,9 @@
       <c r="AE59" s="12"/>
       <c r="AF59" s="12"/>
       <c r="AG59" s="12"/>
-      <c r="AH59" s="12"/>
+      <c r="AH59" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="AI59" s="12"/>
       <c r="AJ59" s="12"/>
       <c r="AK59" s="12"/>
@@ -4853,9 +4882,15 @@
       <c r="BI59" s="12"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
+      <c r="A60" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
@@ -4865,7 +4900,9 @@
       <c r="J60" s="11"/>
       <c r="K60" s="11"/>
       <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
+      <c r="M60" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="N60" s="11"/>
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
@@ -4916,11 +4953,19 @@
       <c r="BI60" s="11"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
+      <c r="A61" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
+      <c r="E61" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
@@ -4979,9 +5024,15 @@
       <c r="BI61" s="12"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="11"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
+      <c r="A62" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
@@ -5010,7 +5061,9 @@
       <c r="AC62" s="11"/>
       <c r="AD62" s="11"/>
       <c r="AE62" s="11"/>
-      <c r="AF62" s="11"/>
+      <c r="AF62" s="11" t="n">
+        <v>40</v>
+      </c>
       <c r="AG62" s="11"/>
       <c r="AH62" s="11"/>
       <c r="AI62" s="11"/>
@@ -5042,9 +5095,15 @@
       <c r="BI62" s="11"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
+      <c r="A63" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
@@ -5061,7 +5120,9 @@
       <c r="Q63" s="12"/>
       <c r="R63" s="12"/>
       <c r="S63" s="12"/>
-      <c r="T63" s="12"/>
+      <c r="T63" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="U63" s="12"/>
       <c r="V63" s="12"/>
       <c r="W63" s="12"/>
@@ -5105,9 +5166,15 @@
       <c r="BI63" s="12"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
+      <c r="A64" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
@@ -5130,7 +5197,9 @@
       <c r="W64" s="11"/>
       <c r="X64" s="11"/>
       <c r="Y64" s="11"/>
-      <c r="Z64" s="11"/>
+      <c r="Z64" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AA64" s="11"/>
       <c r="AB64" s="11"/>
       <c r="AC64" s="11"/>
@@ -5168,9 +5237,15 @@
       <c r="BI64" s="11"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
+      <c r="A65" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
@@ -5178,7 +5253,9 @@
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
-      <c r="K65" s="12"/>
+      <c r="K65" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="L65" s="12"/>
       <c r="M65" s="12"/>
       <c r="N65" s="12"/>
@@ -5231,9 +5308,15 @@
       <c r="BI65" s="12"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
+      <c r="A66" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
@@ -5294,9 +5377,15 @@
       <c r="BI66" s="11"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
+      <c r="A67" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
@@ -5316,7 +5405,9 @@
       <c r="T67" s="12"/>
       <c r="U67" s="12"/>
       <c r="V67" s="12"/>
-      <c r="W67" s="12"/>
+      <c r="W67" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="X67" s="12"/>
       <c r="Y67" s="12"/>
       <c r="Z67" s="12"/>
@@ -5357,9 +5448,15 @@
       <c r="BI67" s="12"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="11"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
+      <c r="A68" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
@@ -5396,7 +5493,9 @@
       <c r="AK68" s="11"/>
       <c r="AL68" s="11"/>
       <c r="AM68" s="11"/>
-      <c r="AN68" s="11"/>
+      <c r="AN68" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="AO68" s="11"/>
       <c r="AP68" s="11"/>
       <c r="AQ68" s="11"/>
@@ -5420,9 +5519,15 @@
       <c r="BI68" s="11"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
+      <c r="A69" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C69" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
       <c r="F69" s="12"/>
@@ -5441,7 +5546,9 @@
       <c r="S69" s="12"/>
       <c r="T69" s="12"/>
       <c r="U69" s="12"/>
-      <c r="V69" s="12"/>
+      <c r="V69" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="W69" s="12"/>
       <c r="X69" s="12"/>
       <c r="Y69" s="12"/>
@@ -5483,9 +5590,15 @@
       <c r="BI69" s="12"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="11"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
+      <c r="A70" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -5510,7 +5623,9 @@
       <c r="Y70" s="11"/>
       <c r="Z70" s="11"/>
       <c r="AA70" s="11"/>
-      <c r="AB70" s="11"/>
+      <c r="AB70" s="11" t="n">
+        <v>5</v>
+      </c>
       <c r="AC70" s="11"/>
       <c r="AD70" s="11"/>
       <c r="AE70" s="11"/>
@@ -5546,14 +5661,22 @@
       <c r="BI70" s="11"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
+      <c r="A71" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C71" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
+      <c r="H71" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
       <c r="K71" s="12"/>
@@ -5609,9 +5732,15 @@
       <c r="BI71" s="12"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="11"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
+      <c r="A72" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C72" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
@@ -5640,7 +5769,9 @@
       <c r="AC72" s="11"/>
       <c r="AD72" s="11"/>
       <c r="AE72" s="11"/>
-      <c r="AF72" s="11"/>
+      <c r="AF72" s="11" t="n">
+        <v>40</v>
+      </c>
       <c r="AG72" s="11"/>
       <c r="AH72" s="11"/>
       <c r="AI72" s="11"/>
@@ -5672,9 +5803,15 @@
       <c r="BI72" s="11"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
+      <c r="A73" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
@@ -5689,7 +5826,9 @@
       <c r="O73" s="12"/>
       <c r="P73" s="12"/>
       <c r="Q73" s="12"/>
-      <c r="R73" s="12"/>
+      <c r="R73" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="S73" s="12"/>
       <c r="T73" s="12"/>
       <c r="U73" s="12"/>
@@ -5735,9 +5874,15 @@
       <c r="BI73" s="12"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
+      <c r="A74" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B74" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C74" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
       <c r="F74" s="11"/>
@@ -5756,7 +5901,9 @@
       <c r="S74" s="11"/>
       <c r="T74" s="11"/>
       <c r="U74" s="11"/>
-      <c r="V74" s="11"/>
+      <c r="V74" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="W74" s="11"/>
       <c r="X74" s="11"/>
       <c r="Y74" s="11"/>
@@ -5798,9 +5945,15 @@
       <c r="BI74" s="11"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
+      <c r="A75" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B75" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
       <c r="F75" s="12"/>
@@ -5821,7 +5974,9 @@
       <c r="U75" s="12"/>
       <c r="V75" s="12"/>
       <c r="W75" s="12"/>
-      <c r="X75" s="12"/>
+      <c r="X75" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="Y75" s="12"/>
       <c r="Z75" s="12"/>
       <c r="AA75" s="12"/>
@@ -5851,7 +6006,9 @@
       <c r="AY75" s="12"/>
       <c r="AZ75" s="12"/>
       <c r="BA75" s="12"/>
-      <c r="BB75" s="12"/>
+      <c r="BB75" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="BC75" s="12"/>
       <c r="BD75" s="12"/>
       <c r="BE75" s="12"/>
@@ -5861,9 +6018,15 @@
       <c r="BI75" s="12"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="11"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
+      <c r="A76" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C76" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
@@ -5887,7 +6050,9 @@
       <c r="X76" s="11"/>
       <c r="Y76" s="11"/>
       <c r="Z76" s="11"/>
-      <c r="AA76" s="11"/>
+      <c r="AA76" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AB76" s="11"/>
       <c r="AC76" s="11"/>
       <c r="AD76" s="11"/>
@@ -5924,9 +6089,15 @@
       <c r="BI76" s="11"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
+      <c r="A77" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B77" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
       <c r="F77" s="12"/>
@@ -5936,7 +6107,9 @@
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
-      <c r="M77" s="12"/>
+      <c r="M77" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="N77" s="12"/>
       <c r="O77" s="12"/>
       <c r="P77" s="12"/>
@@ -5987,9 +6160,15 @@
       <c r="BI77" s="12"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="11"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
+      <c r="A78" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
@@ -6014,7 +6193,9 @@
       <c r="Y78" s="11"/>
       <c r="Z78" s="11"/>
       <c r="AA78" s="11"/>
-      <c r="AB78" s="11"/>
+      <c r="AB78" s="11" t="n">
+        <v>5</v>
+      </c>
       <c r="AC78" s="11"/>
       <c r="AD78" s="11"/>
       <c r="AE78" s="11"/>
@@ -6050,9 +6231,15 @@
       <c r="BI78" s="11"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
+      <c r="A79" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B79" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C79" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
       <c r="F79" s="12"/>
@@ -6071,7 +6258,9 @@
       <c r="S79" s="12"/>
       <c r="T79" s="12"/>
       <c r="U79" s="12"/>
-      <c r="V79" s="12"/>
+      <c r="V79" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="W79" s="12"/>
       <c r="X79" s="12"/>
       <c r="Y79" s="12"/>
@@ -6113,9 +6302,15 @@
       <c r="BI79" s="12"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="11"/>
-      <c r="B80" s="11"/>
-      <c r="C80" s="11"/>
+      <c r="A80" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B80" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C80" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
       <c r="F80" s="11"/>
@@ -6135,7 +6330,9 @@
       <c r="T80" s="11"/>
       <c r="U80" s="11"/>
       <c r="V80" s="11"/>
-      <c r="W80" s="11"/>
+      <c r="W80" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X80" s="11"/>
       <c r="Y80" s="11"/>
       <c r="Z80" s="11"/>
@@ -6176,9 +6373,15 @@
       <c r="BI80" s="11"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
+      <c r="A81" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B81" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C81" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
       <c r="F81" s="12"/>
@@ -6192,7 +6395,9 @@
       <c r="N81" s="12"/>
       <c r="O81" s="12"/>
       <c r="P81" s="12"/>
-      <c r="Q81" s="12"/>
+      <c r="Q81" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="R81" s="12"/>
       <c r="S81" s="12"/>
       <c r="T81" s="12"/>
@@ -6239,9 +6444,15 @@
       <c r="BI81" s="12"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
+      <c r="A82" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B82" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C82" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
       <c r="F82" s="11"/>
@@ -6270,7 +6481,9 @@
       <c r="AC82" s="11"/>
       <c r="AD82" s="11"/>
       <c r="AE82" s="11"/>
-      <c r="AF82" s="11"/>
+      <c r="AF82" s="11" t="n">
+        <v>40</v>
+      </c>
       <c r="AG82" s="11"/>
       <c r="AH82" s="11"/>
       <c r="AI82" s="11"/>
@@ -6302,9 +6515,15 @@
       <c r="BI82" s="11"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="12"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="12"/>
+      <c r="A83" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B83" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C83" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
       <c r="F83" s="12"/>
@@ -6320,7 +6539,9 @@
       <c r="P83" s="12"/>
       <c r="Q83" s="12"/>
       <c r="R83" s="12"/>
-      <c r="S83" s="12"/>
+      <c r="S83" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="T83" s="12"/>
       <c r="U83" s="12"/>
       <c r="V83" s="12"/>
@@ -6355,7 +6576,9 @@
       <c r="AY83" s="12"/>
       <c r="AZ83" s="12"/>
       <c r="BA83" s="12"/>
-      <c r="BB83" s="12"/>
+      <c r="BB83" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="BC83" s="12"/>
       <c r="BD83" s="12"/>
       <c r="BE83" s="12"/>
@@ -6365,9 +6588,15 @@
       <c r="BI83" s="12"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="11"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="11"/>
+      <c r="A84" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B84" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C84" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
       <c r="F84" s="11"/>
@@ -6397,7 +6626,9 @@
       <c r="AD84" s="11"/>
       <c r="AE84" s="11"/>
       <c r="AF84" s="11"/>
-      <c r="AG84" s="11"/>
+      <c r="AG84" s="11" t="n">
+        <v>3000</v>
+      </c>
       <c r="AH84" s="11"/>
       <c r="AI84" s="11"/>
       <c r="AJ84" s="11"/>
@@ -6428,14 +6659,22 @@
       <c r="BI84" s="11"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="12"/>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
+      <c r="A85" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B85" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C85" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
-      <c r="H85" s="12"/>
+      <c r="H85" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="I85" s="12"/>
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
@@ -6491,9 +6730,15 @@
       <c r="BI85" s="12"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="11"/>
-      <c r="B86" s="11"/>
-      <c r="C86" s="11"/>
+      <c r="A86" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B86" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C86" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
@@ -6513,7 +6758,9 @@
       <c r="T86" s="11"/>
       <c r="U86" s="11"/>
       <c r="V86" s="11"/>
-      <c r="W86" s="11"/>
+      <c r="W86" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X86" s="11"/>
       <c r="Y86" s="11"/>
       <c r="Z86" s="11"/>
@@ -6554,9 +6801,15 @@
       <c r="BI86" s="11"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="12"/>
-      <c r="B87" s="12"/>
-      <c r="C87" s="12"/>
+      <c r="A87" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B87" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C87" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
@@ -6587,7 +6840,9 @@
       <c r="AE87" s="12"/>
       <c r="AF87" s="12"/>
       <c r="AG87" s="12"/>
-      <c r="AH87" s="12"/>
+      <c r="AH87" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="AI87" s="12"/>
       <c r="AJ87" s="12"/>
       <c r="AK87" s="12"/>
@@ -6617,9 +6872,15 @@
       <c r="BI87" s="12"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="11"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
+      <c r="A88" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B88" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C88" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
@@ -6650,7 +6911,9 @@
       <c r="AE88" s="11"/>
       <c r="AF88" s="11"/>
       <c r="AG88" s="11"/>
-      <c r="AH88" s="11"/>
+      <c r="AH88" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="AI88" s="11"/>
       <c r="AJ88" s="11"/>
       <c r="AK88" s="11"/>
@@ -6680,9 +6943,15 @@
       <c r="BI88" s="11"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="12"/>
-      <c r="B89" s="12"/>
-      <c r="C89" s="12"/>
+      <c r="A89" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B89" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C89" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
       <c r="F89" s="12"/>
@@ -6694,7 +6963,9 @@
       <c r="L89" s="12"/>
       <c r="M89" s="12"/>
       <c r="N89" s="12"/>
-      <c r="O89" s="12"/>
+      <c r="O89" s="12" t="n">
+        <v>25</v>
+      </c>
       <c r="P89" s="12"/>
       <c r="Q89" s="12"/>
       <c r="R89" s="12"/>
@@ -6743,9 +7014,15 @@
       <c r="BI89" s="12"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="11"/>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
+      <c r="A90" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B90" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C90" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
@@ -6775,7 +7052,9 @@
       <c r="AD90" s="11"/>
       <c r="AE90" s="11"/>
       <c r="AF90" s="11"/>
-      <c r="AG90" s="11"/>
+      <c r="AG90" s="11" t="n">
+        <v>370</v>
+      </c>
       <c r="AH90" s="11"/>
       <c r="AI90" s="11"/>
       <c r="AJ90" s="11"/>
@@ -6806,11 +7085,19 @@
       <c r="BI90" s="11"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="12"/>
-      <c r="B91" s="12"/>
-      <c r="C91" s="12"/>
+      <c r="A91" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B91" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C91" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D91" s="12"/>
-      <c r="E91" s="12"/>
+      <c r="E91" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
@@ -6869,9 +7156,15 @@
       <c r="BI91" s="12"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="11"/>
-      <c r="B92" s="11"/>
-      <c r="C92" s="11"/>
+      <c r="A92" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B92" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C92" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
       <c r="F92" s="11"/>
@@ -6901,7 +7194,9 @@
       <c r="AD92" s="11"/>
       <c r="AE92" s="11"/>
       <c r="AF92" s="11"/>
-      <c r="AG92" s="11"/>
+      <c r="AG92" s="11" t="n">
+        <v>370</v>
+      </c>
       <c r="AH92" s="11"/>
       <c r="AI92" s="11"/>
       <c r="AJ92" s="11"/>
@@ -6932,9 +7227,15 @@
       <c r="BI92" s="11"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="12"/>
-      <c r="B93" s="12"/>
-      <c r="C93" s="12"/>
+      <c r="A93" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B93" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C93" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
       <c r="F93" s="12"/>
@@ -6961,7 +7262,9 @@
       <c r="AA93" s="12"/>
       <c r="AB93" s="12"/>
       <c r="AC93" s="12"/>
-      <c r="AD93" s="12"/>
+      <c r="AD93" s="12" t="n">
+        <v>3</v>
+      </c>
       <c r="AE93" s="12"/>
       <c r="AF93" s="12"/>
       <c r="AG93" s="12"/>
@@ -6995,9 +7298,15 @@
       <c r="BI93" s="12"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="11"/>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
+      <c r="A94" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B94" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C94" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
       <c r="F94" s="11"/>
@@ -7018,7 +7327,9 @@
       <c r="U94" s="11"/>
       <c r="V94" s="11"/>
       <c r="W94" s="11"/>
-      <c r="X94" s="11"/>
+      <c r="X94" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="Y94" s="11"/>
       <c r="Z94" s="11"/>
       <c r="AA94" s="11"/>
@@ -7058,16 +7369,24 @@
       <c r="BI94" s="11"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="12"/>
-      <c r="B95" s="12"/>
-      <c r="C95" s="12"/>
+      <c r="A95" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B95" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C95" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
       <c r="H95" s="12"/>
       <c r="I95" s="12"/>
-      <c r="J95" s="12"/>
+      <c r="J95" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
       <c r="M95" s="12"/>
@@ -7121,9 +7440,15 @@
       <c r="BI95" s="12"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="11"/>
-      <c r="B96" s="11"/>
-      <c r="C96" s="11"/>
+      <c r="A96" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B96" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C96" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
@@ -7133,7 +7458,9 @@
       <c r="J96" s="11"/>
       <c r="K96" s="11"/>
       <c r="L96" s="11"/>
-      <c r="M96" s="11"/>
+      <c r="M96" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="N96" s="11"/>
       <c r="O96" s="11"/>
       <c r="P96" s="11"/>

</xml_diff>

<commit_message>
Up to 139 drops
</commit_message>
<xml_diff>
--- a/Drops.xlsx
+++ b/Drops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="65">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t xml:space="preserve">2020/3/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/3/23</t>
   </si>
 </sst>
 </file>
@@ -488,8 +491,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ393"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B97" activeCellId="0" sqref="B97"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C141" activeCellId="0" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7511,9 +7514,15 @@
       <c r="BI96" s="11"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="12"/>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
+      <c r="A97" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B97" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C97" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
       <c r="F97" s="12"/>
@@ -7574,9 +7583,15 @@
       <c r="BI97" s="12"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="11"/>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
+      <c r="A98" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B98" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C98" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
@@ -7596,7 +7611,9 @@
       <c r="T98" s="11"/>
       <c r="U98" s="11"/>
       <c r="V98" s="11"/>
-      <c r="W98" s="11"/>
+      <c r="W98" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X98" s="11"/>
       <c r="Y98" s="11"/>
       <c r="Z98" s="11"/>
@@ -7637,9 +7654,15 @@
       <c r="BI98" s="11"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="12"/>
-      <c r="B99" s="12"/>
-      <c r="C99" s="12"/>
+      <c r="A99" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B99" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C99" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D99" s="12"/>
       <c r="E99" s="12"/>
       <c r="F99" s="12"/>
@@ -7669,7 +7692,9 @@
       <c r="AD99" s="12"/>
       <c r="AE99" s="12"/>
       <c r="AF99" s="12"/>
-      <c r="AG99" s="12"/>
+      <c r="AG99" s="12" t="n">
+        <v>370</v>
+      </c>
       <c r="AH99" s="12"/>
       <c r="AI99" s="12"/>
       <c r="AJ99" s="12"/>
@@ -7690,7 +7715,9 @@
       <c r="AY99" s="12"/>
       <c r="AZ99" s="12"/>
       <c r="BA99" s="12"/>
-      <c r="BB99" s="12"/>
+      <c r="BB99" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="BC99" s="12"/>
       <c r="BD99" s="12"/>
       <c r="BE99" s="12"/>
@@ -7700,9 +7727,15 @@
       <c r="BI99" s="12"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="11"/>
-      <c r="B100" s="11"/>
-      <c r="C100" s="11"/>
+      <c r="A100" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B100" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C100" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
@@ -7722,7 +7755,9 @@
       <c r="T100" s="11"/>
       <c r="U100" s="11"/>
       <c r="V100" s="11"/>
-      <c r="W100" s="11"/>
+      <c r="W100" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X100" s="11"/>
       <c r="Y100" s="11"/>
       <c r="Z100" s="11"/>
@@ -7763,9 +7798,15 @@
       <c r="BI100" s="11"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="12"/>
-      <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
+      <c r="A101" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B101" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C101" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
       <c r="F101" s="12"/>
@@ -7786,7 +7827,9 @@
       <c r="U101" s="12"/>
       <c r="V101" s="12"/>
       <c r="W101" s="12"/>
-      <c r="X101" s="12"/>
+      <c r="X101" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="Y101" s="12"/>
       <c r="Z101" s="12"/>
       <c r="AA101" s="12"/>
@@ -7826,9 +7869,15 @@
       <c r="BI101" s="12"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="11"/>
-      <c r="B102" s="11"/>
-      <c r="C102" s="11"/>
+      <c r="A102" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B102" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C102" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
@@ -7851,7 +7900,9 @@
       <c r="W102" s="11"/>
       <c r="X102" s="11"/>
       <c r="Y102" s="11"/>
-      <c r="Z102" s="11"/>
+      <c r="Z102" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AA102" s="11"/>
       <c r="AB102" s="11"/>
       <c r="AC102" s="11"/>
@@ -7889,9 +7940,15 @@
       <c r="BI102" s="11"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="12"/>
-      <c r="B103" s="12"/>
-      <c r="C103" s="12"/>
+      <c r="A103" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B103" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C103" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
       <c r="F103" s="12"/>
@@ -7922,7 +7979,9 @@
       <c r="AE103" s="12"/>
       <c r="AF103" s="12"/>
       <c r="AG103" s="12"/>
-      <c r="AH103" s="12"/>
+      <c r="AH103" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="AI103" s="12"/>
       <c r="AJ103" s="12"/>
       <c r="AK103" s="12"/>
@@ -7952,9 +8011,15 @@
       <c r="BI103" s="12"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="11"/>
-      <c r="B104" s="11"/>
-      <c r="C104" s="11"/>
+      <c r="A104" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B104" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C104" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
       <c r="F104" s="11"/>
@@ -7966,7 +8031,9 @@
       <c r="L104" s="11"/>
       <c r="M104" s="11"/>
       <c r="N104" s="11"/>
-      <c r="O104" s="11"/>
+      <c r="O104" s="11" t="n">
+        <v>25</v>
+      </c>
       <c r="P104" s="11"/>
       <c r="Q104" s="11"/>
       <c r="R104" s="11"/>
@@ -8015,9 +8082,15 @@
       <c r="BI104" s="11"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="12"/>
-      <c r="B105" s="12"/>
-      <c r="C105" s="12"/>
+      <c r="A105" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B105" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C105" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
       <c r="F105" s="12"/>
@@ -8042,7 +8115,9 @@
       <c r="Y105" s="12"/>
       <c r="Z105" s="12"/>
       <c r="AA105" s="12"/>
-      <c r="AB105" s="12"/>
+      <c r="AB105" s="12" t="n">
+        <v>5</v>
+      </c>
       <c r="AC105" s="12"/>
       <c r="AD105" s="12"/>
       <c r="AE105" s="12"/>
@@ -8078,9 +8153,15 @@
       <c r="BI105" s="12"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="11"/>
-      <c r="B106" s="11"/>
-      <c r="C106" s="11"/>
+      <c r="A106" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B106" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C106" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
       <c r="F106" s="11"/>
@@ -8110,7 +8191,9 @@
       <c r="AD106" s="11"/>
       <c r="AE106" s="11"/>
       <c r="AF106" s="11"/>
-      <c r="AG106" s="11"/>
+      <c r="AG106" s="11" t="n">
+        <v>370</v>
+      </c>
       <c r="AH106" s="11"/>
       <c r="AI106" s="11"/>
       <c r="AJ106" s="11"/>
@@ -8141,9 +8224,15 @@
       <c r="BI106" s="11"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="12"/>
-      <c r="B107" s="12"/>
-      <c r="C107" s="12"/>
+      <c r="A107" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B107" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C107" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
       <c r="F107" s="12"/>
@@ -8166,7 +8255,9 @@
       <c r="W107" s="12"/>
       <c r="X107" s="12"/>
       <c r="Y107" s="12"/>
-      <c r="Z107" s="12"/>
+      <c r="Z107" s="12" t="n">
+        <v>75</v>
+      </c>
       <c r="AA107" s="12"/>
       <c r="AB107" s="12"/>
       <c r="AC107" s="12"/>
@@ -8204,14 +8295,22 @@
       <c r="BI107" s="12"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="11"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="11"/>
+      <c r="A108" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B108" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C108" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
       <c r="G108" s="11"/>
-      <c r="H108" s="11"/>
+      <c r="H108" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="I108" s="11"/>
       <c r="J108" s="11"/>
       <c r="K108" s="11"/>
@@ -8267,9 +8366,15 @@
       <c r="BI108" s="11"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="12"/>
-      <c r="B109" s="12"/>
-      <c r="C109" s="12"/>
+      <c r="A109" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B109" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C109" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
       <c r="F109" s="12"/>
@@ -8281,7 +8386,9 @@
       <c r="L109" s="12"/>
       <c r="M109" s="12"/>
       <c r="N109" s="12"/>
-      <c r="O109" s="12"/>
+      <c r="O109" s="12" t="n">
+        <v>25</v>
+      </c>
       <c r="P109" s="12"/>
       <c r="Q109" s="12"/>
       <c r="R109" s="12"/>
@@ -8330,9 +8437,15 @@
       <c r="BI109" s="12"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="11"/>
-      <c r="B110" s="11"/>
-      <c r="C110" s="11"/>
+      <c r="A110" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B110" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C110" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D110" s="11"/>
       <c r="E110" s="11"/>
       <c r="F110" s="11"/>
@@ -8393,9 +8506,15 @@
       <c r="BI110" s="11"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="12"/>
-      <c r="B111" s="12"/>
-      <c r="C111" s="12"/>
+      <c r="A111" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B111" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C111" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
       <c r="F111" s="12"/>
@@ -8456,9 +8575,15 @@
       <c r="BI111" s="12"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="11"/>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
+      <c r="A112" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B112" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C112" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D112" s="11"/>
       <c r="E112" s="11"/>
       <c r="F112" s="11"/>
@@ -8481,7 +8606,9 @@
       <c r="W112" s="11"/>
       <c r="X112" s="11"/>
       <c r="Y112" s="11"/>
-      <c r="Z112" s="11"/>
+      <c r="Z112" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AA112" s="11"/>
       <c r="AB112" s="11"/>
       <c r="AC112" s="11"/>
@@ -8519,9 +8646,15 @@
       <c r="BI112" s="11"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="12"/>
-      <c r="B113" s="12"/>
-      <c r="C113" s="12"/>
+      <c r="A113" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B113" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C113" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D113" s="12"/>
       <c r="E113" s="12"/>
       <c r="F113" s="12"/>
@@ -8549,7 +8682,9 @@
       <c r="AB113" s="12"/>
       <c r="AC113" s="12"/>
       <c r="AD113" s="12"/>
-      <c r="AE113" s="12"/>
+      <c r="AE113" s="12" t="n">
+        <v>40</v>
+      </c>
       <c r="AF113" s="12"/>
       <c r="AG113" s="12"/>
       <c r="AH113" s="12"/>
@@ -8582,9 +8717,15 @@
       <c r="BI113" s="12"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="11"/>
-      <c r="B114" s="11"/>
-      <c r="C114" s="11"/>
+      <c r="A114" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B114" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C114" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
       <c r="F114" s="11"/>
@@ -8614,7 +8755,9 @@
       <c r="AD114" s="11"/>
       <c r="AE114" s="11"/>
       <c r="AF114" s="11"/>
-      <c r="AG114" s="11"/>
+      <c r="AG114" s="11" t="n">
+        <v>370</v>
+      </c>
       <c r="AH114" s="11"/>
       <c r="AI114" s="11"/>
       <c r="AJ114" s="11"/>
@@ -8645,9 +8788,15 @@
       <c r="BI114" s="11"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="12"/>
-      <c r="B115" s="12"/>
-      <c r="C115" s="12"/>
+      <c r="A115" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B115" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C115" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D115" s="12"/>
       <c r="E115" s="12"/>
       <c r="F115" s="12"/>
@@ -8676,7 +8825,9 @@
       <c r="AC115" s="12"/>
       <c r="AD115" s="12"/>
       <c r="AE115" s="12"/>
-      <c r="AF115" s="12"/>
+      <c r="AF115" s="12" t="n">
+        <v>40</v>
+      </c>
       <c r="AG115" s="12"/>
       <c r="AH115" s="12"/>
       <c r="AI115" s="12"/>
@@ -8708,9 +8859,15 @@
       <c r="BI115" s="12"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="11"/>
-      <c r="B116" s="11"/>
-      <c r="C116" s="11"/>
+      <c r="A116" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B116" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C116" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
       <c r="F116" s="11"/>
@@ -8730,7 +8887,9 @@
       <c r="T116" s="11"/>
       <c r="U116" s="11"/>
       <c r="V116" s="11"/>
-      <c r="W116" s="11"/>
+      <c r="W116" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X116" s="11"/>
       <c r="Y116" s="11"/>
       <c r="Z116" s="11"/>
@@ -8771,16 +8930,24 @@
       <c r="BI116" s="11"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="12"/>
-      <c r="B117" s="12"/>
-      <c r="C117" s="12"/>
+      <c r="A117" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B117" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C117" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D117" s="12"/>
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
       <c r="G117" s="12"/>
       <c r="H117" s="12"/>
       <c r="I117" s="12"/>
-      <c r="J117" s="12"/>
+      <c r="J117" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="K117" s="12"/>
       <c r="L117" s="12"/>
       <c r="M117" s="12"/>
@@ -8834,9 +9001,15 @@
       <c r="BI117" s="12"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="11"/>
-      <c r="B118" s="11"/>
-      <c r="C118" s="11"/>
+      <c r="A118" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B118" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C118" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
       <c r="F118" s="11"/>
@@ -8860,7 +9033,9 @@
       <c r="X118" s="11"/>
       <c r="Y118" s="11"/>
       <c r="Z118" s="11"/>
-      <c r="AA118" s="11"/>
+      <c r="AA118" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AB118" s="11"/>
       <c r="AC118" s="11"/>
       <c r="AD118" s="11"/>
@@ -8897,9 +9072,15 @@
       <c r="BI118" s="11"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="12"/>
-      <c r="B119" s="12"/>
-      <c r="C119" s="12"/>
+      <c r="A119" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B119" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C119" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D119" s="12"/>
       <c r="E119" s="12"/>
       <c r="F119" s="12"/>
@@ -8960,9 +9141,15 @@
       <c r="BI119" s="12"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="11"/>
-      <c r="B120" s="11"/>
-      <c r="C120" s="11"/>
+      <c r="A120" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B120" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C120" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D120" s="11"/>
       <c r="E120" s="11"/>
       <c r="F120" s="11"/>
@@ -8980,7 +9167,9 @@
       <c r="R120" s="11"/>
       <c r="S120" s="11"/>
       <c r="T120" s="11"/>
-      <c r="U120" s="11"/>
+      <c r="U120" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="V120" s="11"/>
       <c r="W120" s="11"/>
       <c r="X120" s="11"/>
@@ -9023,16 +9212,24 @@
       <c r="BI120" s="11"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="12"/>
-      <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
+      <c r="A121" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B121" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C121" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D121" s="12"/>
       <c r="E121" s="12"/>
       <c r="F121" s="12"/>
       <c r="G121" s="12"/>
       <c r="H121" s="12"/>
       <c r="I121" s="12"/>
-      <c r="J121" s="12"/>
+      <c r="J121" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="K121" s="12"/>
       <c r="L121" s="12"/>
       <c r="M121" s="12"/>
@@ -9086,9 +9283,15 @@
       <c r="BI121" s="12"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="11"/>
-      <c r="B122" s="11"/>
-      <c r="C122" s="11"/>
+      <c r="A122" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B122" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C122" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D122" s="11"/>
       <c r="E122" s="11"/>
       <c r="F122" s="11"/>
@@ -9118,7 +9321,9 @@
       <c r="AD122" s="11"/>
       <c r="AE122" s="11"/>
       <c r="AF122" s="11"/>
-      <c r="AG122" s="11"/>
+      <c r="AG122" s="11" t="n">
+        <v>370</v>
+      </c>
       <c r="AH122" s="11"/>
       <c r="AI122" s="11"/>
       <c r="AJ122" s="11"/>
@@ -9149,9 +9354,15 @@
       <c r="BI122" s="11"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="12"/>
-      <c r="B123" s="12"/>
-      <c r="C123" s="12"/>
+      <c r="A123" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B123" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C123" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D123" s="12"/>
       <c r="E123" s="12"/>
       <c r="F123" s="12"/>
@@ -9181,7 +9392,9 @@
       <c r="AD123" s="12"/>
       <c r="AE123" s="12"/>
       <c r="AF123" s="12"/>
-      <c r="AG123" s="12"/>
+      <c r="AG123" s="12" t="n">
+        <v>370</v>
+      </c>
       <c r="AH123" s="12"/>
       <c r="AI123" s="12"/>
       <c r="AJ123" s="12"/>
@@ -9212,14 +9425,22 @@
       <c r="BI123" s="12"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="11"/>
-      <c r="B124" s="11"/>
-      <c r="C124" s="11"/>
+      <c r="A124" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B124" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C124" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D124" s="11"/>
       <c r="E124" s="11"/>
       <c r="F124" s="11"/>
       <c r="G124" s="11"/>
-      <c r="H124" s="11"/>
+      <c r="H124" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="I124" s="11"/>
       <c r="J124" s="11"/>
       <c r="K124" s="11"/>
@@ -9265,7 +9486,9 @@
       <c r="AY124" s="11"/>
       <c r="AZ124" s="11"/>
       <c r="BA124" s="11"/>
-      <c r="BB124" s="11"/>
+      <c r="BB124" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="BC124" s="11"/>
       <c r="BD124" s="11"/>
       <c r="BE124" s="11"/>
@@ -9275,9 +9498,15 @@
       <c r="BI124" s="11"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="12"/>
-      <c r="B125" s="12"/>
-      <c r="C125" s="12"/>
+      <c r="A125" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B125" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C125" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D125" s="12"/>
       <c r="E125" s="12"/>
       <c r="F125" s="12"/>
@@ -9307,7 +9536,9 @@
       <c r="AD125" s="12"/>
       <c r="AE125" s="12"/>
       <c r="AF125" s="12"/>
-      <c r="AG125" s="12"/>
+      <c r="AG125" s="12" t="n">
+        <v>370</v>
+      </c>
       <c r="AH125" s="12"/>
       <c r="AI125" s="12"/>
       <c r="AJ125" s="12"/>
@@ -9338,9 +9569,15 @@
       <c r="BI125" s="12"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="11"/>
-      <c r="B126" s="11"/>
-      <c r="C126" s="11"/>
+      <c r="A126" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B126" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C126" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D126" s="11"/>
       <c r="E126" s="11"/>
       <c r="F126" s="11"/>
@@ -9364,7 +9601,9 @@
       <c r="X126" s="11"/>
       <c r="Y126" s="11"/>
       <c r="Z126" s="11"/>
-      <c r="AA126" s="11"/>
+      <c r="AA126" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AB126" s="11"/>
       <c r="AC126" s="11"/>
       <c r="AD126" s="11"/>
@@ -9401,9 +9640,15 @@
       <c r="BI126" s="11"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="12"/>
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
+      <c r="A127" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B127" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C127" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D127" s="12"/>
       <c r="E127" s="12"/>
       <c r="F127" s="12"/>
@@ -9428,7 +9673,9 @@
       <c r="Y127" s="12"/>
       <c r="Z127" s="12"/>
       <c r="AA127" s="12"/>
-      <c r="AB127" s="12"/>
+      <c r="AB127" s="12" t="n">
+        <v>5</v>
+      </c>
       <c r="AC127" s="12"/>
       <c r="AD127" s="12"/>
       <c r="AE127" s="12"/>
@@ -9464,9 +9711,15 @@
       <c r="BI127" s="12"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="11"/>
-      <c r="B128" s="11"/>
-      <c r="C128" s="11"/>
+      <c r="A128" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B128" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C128" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
       <c r="F128" s="11"/>
@@ -9489,7 +9742,9 @@
       <c r="W128" s="11"/>
       <c r="X128" s="11"/>
       <c r="Y128" s="11"/>
-      <c r="Z128" s="11"/>
+      <c r="Z128" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AA128" s="11"/>
       <c r="AB128" s="11"/>
       <c r="AC128" s="11"/>
@@ -9527,14 +9782,22 @@
       <c r="BI128" s="11"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="12"/>
-      <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
+      <c r="A129" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B129" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C129" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D129" s="12"/>
       <c r="E129" s="12"/>
       <c r="F129" s="12"/>
       <c r="G129" s="12"/>
-      <c r="H129" s="12"/>
+      <c r="H129" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="I129" s="12"/>
       <c r="J129" s="12"/>
       <c r="K129" s="12"/>
@@ -9590,9 +9853,15 @@
       <c r="BI129" s="12"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="11"/>
-      <c r="B130" s="11"/>
-      <c r="C130" s="11"/>
+      <c r="A130" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B130" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C130" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D130" s="11"/>
       <c r="E130" s="11"/>
       <c r="F130" s="11"/>
@@ -9614,7 +9883,9 @@
       <c r="V130" s="11"/>
       <c r="W130" s="11"/>
       <c r="X130" s="11"/>
-      <c r="Y130" s="11"/>
+      <c r="Y130" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="Z130" s="11"/>
       <c r="AA130" s="11"/>
       <c r="AB130" s="11"/>
@@ -9653,9 +9924,15 @@
       <c r="BI130" s="11"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="12"/>
-      <c r="B131" s="12"/>
-      <c r="C131" s="12"/>
+      <c r="A131" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B131" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C131" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D131" s="12"/>
       <c r="E131" s="12"/>
       <c r="F131" s="12"/>
@@ -9665,7 +9942,9 @@
       <c r="J131" s="12"/>
       <c r="K131" s="12"/>
       <c r="L131" s="12"/>
-      <c r="M131" s="12"/>
+      <c r="M131" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="N131" s="12"/>
       <c r="O131" s="12"/>
       <c r="P131" s="12"/>
@@ -9706,7 +9985,9 @@
       <c r="AY131" s="12"/>
       <c r="AZ131" s="12"/>
       <c r="BA131" s="12"/>
-      <c r="BB131" s="12"/>
+      <c r="BB131" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="BC131" s="12"/>
       <c r="BD131" s="12"/>
       <c r="BE131" s="12"/>
@@ -9716,9 +9997,15 @@
       <c r="BI131" s="12"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="11"/>
-      <c r="B132" s="11"/>
-      <c r="C132" s="11"/>
+      <c r="A132" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B132" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C132" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D132" s="11"/>
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
@@ -9728,7 +10015,9 @@
       <c r="J132" s="11"/>
       <c r="K132" s="11"/>
       <c r="L132" s="11"/>
-      <c r="M132" s="11"/>
+      <c r="M132" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="N132" s="11"/>
       <c r="O132" s="11"/>
       <c r="P132" s="11"/>
@@ -9769,7 +10058,9 @@
       <c r="AY132" s="11"/>
       <c r="AZ132" s="11"/>
       <c r="BA132" s="11"/>
-      <c r="BB132" s="11"/>
+      <c r="BB132" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="BC132" s="11"/>
       <c r="BD132" s="11"/>
       <c r="BE132" s="11"/>
@@ -9779,9 +10070,15 @@
       <c r="BI132" s="11"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="12"/>
-      <c r="B133" s="12"/>
-      <c r="C133" s="12"/>
+      <c r="A133" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B133" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C133" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D133" s="12"/>
       <c r="E133" s="12"/>
       <c r="F133" s="12"/>
@@ -9842,9 +10139,15 @@
       <c r="BI133" s="12"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="11"/>
-      <c r="B134" s="11"/>
-      <c r="C134" s="11"/>
+      <c r="A134" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B134" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C134" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D134" s="11"/>
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
@@ -9867,12 +10170,16 @@
       <c r="W134" s="11"/>
       <c r="X134" s="11"/>
       <c r="Y134" s="11"/>
-      <c r="Z134" s="11"/>
+      <c r="Z134" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AA134" s="11"/>
       <c r="AB134" s="11"/>
       <c r="AC134" s="11"/>
       <c r="AD134" s="11"/>
-      <c r="AE134" s="11"/>
+      <c r="AE134" s="11" t="n">
+        <v>40</v>
+      </c>
       <c r="AF134" s="11"/>
       <c r="AG134" s="11"/>
       <c r="AH134" s="11"/>
@@ -9905,9 +10212,15 @@
       <c r="BI134" s="11"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="12"/>
-      <c r="B135" s="12"/>
-      <c r="C135" s="12"/>
+      <c r="A135" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B135" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C135" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D135" s="12"/>
       <c r="E135" s="12"/>
       <c r="F135" s="12"/>
@@ -9932,7 +10245,9 @@
       <c r="Y135" s="12"/>
       <c r="Z135" s="12"/>
       <c r="AA135" s="12"/>
-      <c r="AB135" s="12"/>
+      <c r="AB135" s="12" t="n">
+        <v>5</v>
+      </c>
       <c r="AC135" s="12"/>
       <c r="AD135" s="12"/>
       <c r="AE135" s="12"/>
@@ -9968,9 +10283,15 @@
       <c r="BI135" s="12"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="11"/>
-      <c r="B136" s="11"/>
-      <c r="C136" s="11"/>
+      <c r="A136" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B136" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C136" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D136" s="11"/>
       <c r="E136" s="11"/>
       <c r="F136" s="11"/>
@@ -9990,7 +10311,9 @@
       <c r="T136" s="11"/>
       <c r="U136" s="11"/>
       <c r="V136" s="11"/>
-      <c r="W136" s="11"/>
+      <c r="W136" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X136" s="11"/>
       <c r="Y136" s="11"/>
       <c r="Z136" s="11"/>
@@ -10021,7 +10344,9 @@
       <c r="AY136" s="11"/>
       <c r="AZ136" s="11"/>
       <c r="BA136" s="11"/>
-      <c r="BB136" s="11"/>
+      <c r="BB136" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="BC136" s="11"/>
       <c r="BD136" s="11"/>
       <c r="BE136" s="11"/>
@@ -10031,9 +10356,15 @@
       <c r="BI136" s="11"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="12"/>
-      <c r="B137" s="12"/>
-      <c r="C137" s="12"/>
+      <c r="A137" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B137" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C137" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D137" s="12"/>
       <c r="E137" s="12"/>
       <c r="F137" s="12"/>
@@ -10064,7 +10395,9 @@
       <c r="AE137" s="12"/>
       <c r="AF137" s="12"/>
       <c r="AG137" s="12"/>
-      <c r="AH137" s="12"/>
+      <c r="AH137" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="AI137" s="12"/>
       <c r="AJ137" s="12"/>
       <c r="AK137" s="12"/>
@@ -10094,9 +10427,15 @@
       <c r="BI137" s="12"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="11"/>
-      <c r="B138" s="11"/>
-      <c r="C138" s="11"/>
+      <c r="A138" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B138" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C138" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
       <c r="F138" s="11"/>
@@ -10116,7 +10455,9 @@
       <c r="T138" s="11"/>
       <c r="U138" s="11"/>
       <c r="V138" s="11"/>
-      <c r="W138" s="11"/>
+      <c r="W138" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X138" s="11"/>
       <c r="Y138" s="11"/>
       <c r="Z138" s="11"/>
@@ -10157,9 +10498,15 @@
       <c r="BI138" s="11"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="12"/>
-      <c r="B139" s="12"/>
-      <c r="C139" s="12"/>
+      <c r="A139" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B139" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C139" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D139" s="12"/>
       <c r="E139" s="12"/>
       <c r="F139" s="12"/>
@@ -10190,7 +10537,9 @@
       <c r="AE139" s="12"/>
       <c r="AF139" s="12"/>
       <c r="AG139" s="12"/>
-      <c r="AH139" s="12"/>
+      <c r="AH139" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="AI139" s="12"/>
       <c r="AJ139" s="12"/>
       <c r="AK139" s="12"/>
@@ -10220,9 +10569,15 @@
       <c r="BI139" s="12"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="11"/>
-      <c r="B140" s="11"/>
-      <c r="C140" s="11"/>
+      <c r="A140" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B140" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C140" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
       <c r="F140" s="11"/>
@@ -10242,7 +10597,9 @@
       <c r="T140" s="11"/>
       <c r="U140" s="11"/>
       <c r="V140" s="11"/>
-      <c r="W140" s="11"/>
+      <c r="W140" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X140" s="11"/>
       <c r="Y140" s="11"/>
       <c r="Z140" s="11"/>

</xml_diff>

<commit_message>
Up to 174 drops
</commit_message>
<xml_diff>
--- a/Drops.xlsx
+++ b/Drops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="66">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t xml:space="preserve">2020/3/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/3/24</t>
   </si>
 </sst>
 </file>
@@ -491,8 +494,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ393"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C141" activeCellId="0" sqref="C141"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B175" activeCellId="0" sqref="B175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10640,9 +10643,15 @@
       <c r="BI140" s="11"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="12"/>
-      <c r="B141" s="12"/>
-      <c r="C141" s="12"/>
+      <c r="A141" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B141" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C141" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D141" s="12"/>
       <c r="E141" s="12"/>
       <c r="F141" s="12"/>
@@ -10670,7 +10679,9 @@
       <c r="AB141" s="12"/>
       <c r="AC141" s="12"/>
       <c r="AD141" s="12"/>
-      <c r="AE141" s="12"/>
+      <c r="AE141" s="12" t="n">
+        <v>40</v>
+      </c>
       <c r="AF141" s="12"/>
       <c r="AG141" s="12"/>
       <c r="AH141" s="12"/>
@@ -10703,9 +10714,15 @@
       <c r="BI141" s="12"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="11"/>
-      <c r="B142" s="11"/>
-      <c r="C142" s="11"/>
+      <c r="A142" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B142" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C142" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
       <c r="F142" s="11"/>
@@ -10725,7 +10742,9 @@
       <c r="T142" s="11"/>
       <c r="U142" s="11"/>
       <c r="V142" s="11"/>
-      <c r="W142" s="11"/>
+      <c r="W142" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X142" s="11"/>
       <c r="Y142" s="11"/>
       <c r="Z142" s="11"/>
@@ -10766,9 +10785,15 @@
       <c r="BI142" s="11"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="12"/>
-      <c r="B143" s="12"/>
-      <c r="C143" s="12"/>
+      <c r="A143" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B143" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C143" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D143" s="12"/>
       <c r="E143" s="12"/>
       <c r="F143" s="12"/>
@@ -10796,7 +10821,9 @@
       <c r="AB143" s="12"/>
       <c r="AC143" s="12"/>
       <c r="AD143" s="12"/>
-      <c r="AE143" s="12"/>
+      <c r="AE143" s="12" t="n">
+        <v>40</v>
+      </c>
       <c r="AF143" s="12"/>
       <c r="AG143" s="12"/>
       <c r="AH143" s="12"/>
@@ -10829,9 +10856,15 @@
       <c r="BI143" s="12"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="11"/>
-      <c r="B144" s="11"/>
-      <c r="C144" s="11"/>
+      <c r="A144" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B144" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C144" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
       <c r="F144" s="11"/>
@@ -10852,7 +10885,9 @@
       <c r="U144" s="11"/>
       <c r="V144" s="11"/>
       <c r="W144" s="11"/>
-      <c r="X144" s="11"/>
+      <c r="X144" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="Y144" s="11"/>
       <c r="Z144" s="11"/>
       <c r="AA144" s="11"/>
@@ -10892,14 +10927,22 @@
       <c r="BI144" s="11"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="12"/>
-      <c r="B145" s="12"/>
-      <c r="C145" s="12"/>
+      <c r="A145" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B145" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C145" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D145" s="12"/>
       <c r="E145" s="12"/>
       <c r="F145" s="12"/>
       <c r="G145" s="12"/>
-      <c r="H145" s="12"/>
+      <c r="H145" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="I145" s="12"/>
       <c r="J145" s="12"/>
       <c r="K145" s="12"/>
@@ -10955,9 +10998,15 @@
       <c r="BI145" s="12"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="11"/>
-      <c r="B146" s="11"/>
-      <c r="C146" s="11"/>
+      <c r="A146" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B146" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C146" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
       <c r="F146" s="11"/>
@@ -10979,7 +11028,9 @@
       <c r="V146" s="11"/>
       <c r="W146" s="11"/>
       <c r="X146" s="11"/>
-      <c r="Y146" s="11"/>
+      <c r="Y146" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="Z146" s="11"/>
       <c r="AA146" s="11"/>
       <c r="AB146" s="11"/>
@@ -11018,9 +11069,15 @@
       <c r="BI146" s="11"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="12"/>
-      <c r="B147" s="12"/>
-      <c r="C147" s="12"/>
+      <c r="A147" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B147" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C147" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D147" s="12"/>
       <c r="E147" s="12"/>
       <c r="F147" s="12"/>
@@ -11044,7 +11101,9 @@
       <c r="X147" s="12"/>
       <c r="Y147" s="12"/>
       <c r="Z147" s="12"/>
-      <c r="AA147" s="12"/>
+      <c r="AA147" s="12" t="n">
+        <v>75</v>
+      </c>
       <c r="AB147" s="12"/>
       <c r="AC147" s="12"/>
       <c r="AD147" s="12"/>
@@ -11081,9 +11140,15 @@
       <c r="BI147" s="12"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="11"/>
-      <c r="B148" s="11"/>
-      <c r="C148" s="11"/>
+      <c r="A148" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B148" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C148" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
       <c r="F148" s="11"/>
@@ -11102,7 +11167,9 @@
       <c r="S148" s="11"/>
       <c r="T148" s="11"/>
       <c r="U148" s="11"/>
-      <c r="V148" s="11"/>
+      <c r="V148" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="W148" s="11"/>
       <c r="X148" s="11"/>
       <c r="Y148" s="11"/>
@@ -11144,9 +11211,15 @@
       <c r="BI148" s="11"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="12"/>
-      <c r="B149" s="12"/>
-      <c r="C149" s="12"/>
+      <c r="A149" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B149" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C149" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D149" s="12"/>
       <c r="E149" s="12"/>
       <c r="F149" s="12"/>
@@ -11156,7 +11229,9 @@
       <c r="J149" s="12"/>
       <c r="K149" s="12"/>
       <c r="L149" s="12"/>
-      <c r="M149" s="12"/>
+      <c r="M149" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="N149" s="12"/>
       <c r="O149" s="12"/>
       <c r="P149" s="12"/>
@@ -11207,9 +11282,15 @@
       <c r="BI149" s="12"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="11"/>
-      <c r="B150" s="11"/>
-      <c r="C150" s="11"/>
+      <c r="A150" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B150" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C150" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
       <c r="F150" s="11"/>
@@ -11230,7 +11311,9 @@
       <c r="U150" s="11"/>
       <c r="V150" s="11"/>
       <c r="W150" s="11"/>
-      <c r="X150" s="11"/>
+      <c r="X150" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="Y150" s="11"/>
       <c r="Z150" s="11"/>
       <c r="AA150" s="11"/>
@@ -11270,9 +11353,15 @@
       <c r="BI150" s="11"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="12"/>
-      <c r="B151" s="12"/>
-      <c r="C151" s="12"/>
+      <c r="A151" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B151" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C151" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D151" s="12"/>
       <c r="E151" s="12"/>
       <c r="F151" s="12"/>
@@ -11296,7 +11385,9 @@
       <c r="X151" s="12"/>
       <c r="Y151" s="12"/>
       <c r="Z151" s="12"/>
-      <c r="AA151" s="12"/>
+      <c r="AA151" s="12" t="n">
+        <v>75</v>
+      </c>
       <c r="AB151" s="12"/>
       <c r="AC151" s="12"/>
       <c r="AD151" s="12"/>
@@ -11333,16 +11424,24 @@
       <c r="BI151" s="12"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="11"/>
-      <c r="B152" s="11"/>
-      <c r="C152" s="11"/>
+      <c r="A152" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B152" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C152" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
       <c r="F152" s="11"/>
       <c r="G152" s="11"/>
       <c r="H152" s="11"/>
       <c r="I152" s="11"/>
-      <c r="J152" s="11"/>
+      <c r="J152" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="K152" s="11"/>
       <c r="L152" s="11"/>
       <c r="M152" s="11"/>
@@ -11396,9 +11495,15 @@
       <c r="BI152" s="11"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="12"/>
-      <c r="B153" s="12"/>
-      <c r="C153" s="12"/>
+      <c r="A153" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B153" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C153" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D153" s="12"/>
       <c r="E153" s="12"/>
       <c r="F153" s="12"/>
@@ -11411,7 +11516,9 @@
       <c r="M153" s="12"/>
       <c r="N153" s="12"/>
       <c r="O153" s="12"/>
-      <c r="P153" s="12"/>
+      <c r="P153" s="12" t="n">
+        <v>30</v>
+      </c>
       <c r="Q153" s="12"/>
       <c r="R153" s="12"/>
       <c r="S153" s="12"/>
@@ -11459,9 +11566,15 @@
       <c r="BI153" s="12"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="11"/>
-      <c r="B154" s="11"/>
-      <c r="C154" s="11"/>
+      <c r="A154" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B154" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C154" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
       <c r="F154" s="11"/>
@@ -11479,7 +11592,9 @@
       <c r="R154" s="11"/>
       <c r="S154" s="11"/>
       <c r="T154" s="11"/>
-      <c r="U154" s="11"/>
+      <c r="U154" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="V154" s="11"/>
       <c r="W154" s="11"/>
       <c r="X154" s="11"/>
@@ -11522,9 +11637,15 @@
       <c r="BI154" s="11"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="12"/>
-      <c r="B155" s="12"/>
-      <c r="C155" s="12"/>
+      <c r="A155" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B155" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C155" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D155" s="12"/>
       <c r="E155" s="12"/>
       <c r="F155" s="12"/>
@@ -11543,7 +11664,9 @@
       <c r="S155" s="12"/>
       <c r="T155" s="12"/>
       <c r="U155" s="12"/>
-      <c r="V155" s="12"/>
+      <c r="V155" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="W155" s="12"/>
       <c r="X155" s="12"/>
       <c r="Y155" s="12"/>
@@ -11585,9 +11708,15 @@
       <c r="BI155" s="12"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="11"/>
-      <c r="B156" s="11"/>
-      <c r="C156" s="11"/>
+      <c r="A156" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B156" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C156" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D156" s="11"/>
       <c r="E156" s="11"/>
       <c r="F156" s="11"/>
@@ -11596,7 +11725,9 @@
       <c r="I156" s="11"/>
       <c r="J156" s="11"/>
       <c r="K156" s="11"/>
-      <c r="L156" s="11"/>
+      <c r="L156" s="11" t="n">
+        <v>20</v>
+      </c>
       <c r="M156" s="11"/>
       <c r="N156" s="11"/>
       <c r="O156" s="11"/>
@@ -11648,9 +11779,15 @@
       <c r="BI156" s="11"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="12"/>
-      <c r="B157" s="12"/>
-      <c r="C157" s="12"/>
+      <c r="A157" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B157" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C157" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D157" s="12"/>
       <c r="E157" s="12"/>
       <c r="F157" s="12"/>
@@ -11677,7 +11814,9 @@
       <c r="AA157" s="12"/>
       <c r="AB157" s="12"/>
       <c r="AC157" s="12"/>
-      <c r="AD157" s="12"/>
+      <c r="AD157" s="12" t="n">
+        <v>3</v>
+      </c>
       <c r="AE157" s="12"/>
       <c r="AF157" s="12"/>
       <c r="AG157" s="12"/>
@@ -11706,14 +11845,22 @@
       <c r="BD157" s="12"/>
       <c r="BE157" s="12"/>
       <c r="BF157" s="12"/>
-      <c r="BG157" s="12"/>
+      <c r="BG157" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="BH157" s="12"/>
       <c r="BI157" s="12"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="11"/>
-      <c r="B158" s="11"/>
-      <c r="C158" s="11"/>
+      <c r="A158" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B158" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C158" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
       <c r="F158" s="11"/>
@@ -11722,7 +11869,9 @@
       <c r="I158" s="11"/>
       <c r="J158" s="11"/>
       <c r="K158" s="11"/>
-      <c r="L158" s="11"/>
+      <c r="L158" s="11" t="n">
+        <v>20</v>
+      </c>
       <c r="M158" s="11"/>
       <c r="N158" s="11"/>
       <c r="O158" s="11"/>
@@ -11774,9 +11923,15 @@
       <c r="BI158" s="11"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="12"/>
-      <c r="B159" s="12"/>
-      <c r="C159" s="12"/>
+      <c r="A159" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B159" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C159" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D159" s="12"/>
       <c r="E159" s="12"/>
       <c r="F159" s="12"/>
@@ -11795,7 +11950,9 @@
       <c r="S159" s="12"/>
       <c r="T159" s="12"/>
       <c r="U159" s="12"/>
-      <c r="V159" s="12"/>
+      <c r="V159" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="W159" s="12"/>
       <c r="X159" s="12"/>
       <c r="Y159" s="12"/>
@@ -11837,9 +11994,15 @@
       <c r="BI159" s="12"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="11"/>
-      <c r="B160" s="11"/>
-      <c r="C160" s="11"/>
+      <c r="A160" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B160" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C160" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
       <c r="F160" s="11"/>
@@ -11866,7 +12029,9 @@
       <c r="AA160" s="11"/>
       <c r="AB160" s="11"/>
       <c r="AC160" s="11"/>
-      <c r="AD160" s="11"/>
+      <c r="AD160" s="11" t="n">
+        <v>3</v>
+      </c>
       <c r="AE160" s="11"/>
       <c r="AF160" s="11"/>
       <c r="AG160" s="11"/>
@@ -11900,9 +12065,15 @@
       <c r="BI160" s="11"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="12"/>
-      <c r="B161" s="12"/>
-      <c r="C161" s="12"/>
+      <c r="A161" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B161" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C161" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D161" s="12"/>
       <c r="E161" s="12"/>
       <c r="F161" s="12"/>
@@ -11933,7 +12104,9 @@
       <c r="AE161" s="12"/>
       <c r="AF161" s="12"/>
       <c r="AG161" s="12"/>
-      <c r="AH161" s="12"/>
+      <c r="AH161" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="AI161" s="12"/>
       <c r="AJ161" s="12"/>
       <c r="AK161" s="12"/>
@@ -11963,9 +12136,15 @@
       <c r="BI161" s="12"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="11"/>
-      <c r="B162" s="11"/>
-      <c r="C162" s="11"/>
+      <c r="A162" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B162" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C162" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
       <c r="F162" s="11"/>
@@ -11987,7 +12166,9 @@
       <c r="V162" s="11"/>
       <c r="W162" s="11"/>
       <c r="X162" s="11"/>
-      <c r="Y162" s="11"/>
+      <c r="Y162" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="Z162" s="11"/>
       <c r="AA162" s="11"/>
       <c r="AB162" s="11"/>
@@ -12026,9 +12207,15 @@
       <c r="BI162" s="11"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="12"/>
-      <c r="B163" s="12"/>
-      <c r="C163" s="12"/>
+      <c r="A163" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B163" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C163" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D163" s="12"/>
       <c r="E163" s="12"/>
       <c r="F163" s="12"/>
@@ -12046,7 +12233,9 @@
       <c r="R163" s="12"/>
       <c r="S163" s="12"/>
       <c r="T163" s="12"/>
-      <c r="U163" s="12"/>
+      <c r="U163" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="V163" s="12"/>
       <c r="W163" s="12"/>
       <c r="X163" s="12"/>
@@ -12089,9 +12278,15 @@
       <c r="BI163" s="12"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="11"/>
-      <c r="B164" s="11"/>
-      <c r="C164" s="11"/>
+      <c r="A164" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B164" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C164" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
       <c r="F164" s="11"/>
@@ -12115,7 +12310,9 @@
       <c r="X164" s="11"/>
       <c r="Y164" s="11"/>
       <c r="Z164" s="11"/>
-      <c r="AA164" s="11"/>
+      <c r="AA164" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AB164" s="11"/>
       <c r="AC164" s="11"/>
       <c r="AD164" s="11"/>
@@ -12152,9 +12349,15 @@
       <c r="BI164" s="11"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="12"/>
-      <c r="B165" s="12"/>
-      <c r="C165" s="12"/>
+      <c r="A165" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B165" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C165" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D165" s="12"/>
       <c r="E165" s="12"/>
       <c r="F165" s="12"/>
@@ -12175,7 +12378,9 @@
       <c r="U165" s="12"/>
       <c r="V165" s="12"/>
       <c r="W165" s="12"/>
-      <c r="X165" s="12"/>
+      <c r="X165" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="Y165" s="12"/>
       <c r="Z165" s="12"/>
       <c r="AA165" s="12"/>
@@ -12215,9 +12420,15 @@
       <c r="BI165" s="12"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="11"/>
-      <c r="B166" s="11"/>
-      <c r="C166" s="11"/>
+      <c r="A166" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B166" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C166" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
       <c r="F166" s="11"/>
@@ -12248,7 +12459,9 @@
       <c r="AE166" s="11"/>
       <c r="AF166" s="11"/>
       <c r="AG166" s="11"/>
-      <c r="AH166" s="11"/>
+      <c r="AH166" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="AI166" s="11"/>
       <c r="AJ166" s="11"/>
       <c r="AK166" s="11"/>
@@ -12278,9 +12491,15 @@
       <c r="BI166" s="11"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="12"/>
-      <c r="B167" s="12"/>
-      <c r="C167" s="12"/>
+      <c r="A167" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B167" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C167" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D167" s="12"/>
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
@@ -12299,7 +12518,9 @@
       <c r="S167" s="12"/>
       <c r="T167" s="12"/>
       <c r="U167" s="12"/>
-      <c r="V167" s="12"/>
+      <c r="V167" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="W167" s="12"/>
       <c r="X167" s="12"/>
       <c r="Y167" s="12"/>
@@ -12341,9 +12562,15 @@
       <c r="BI167" s="12"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="11"/>
-      <c r="B168" s="11"/>
-      <c r="C168" s="11"/>
+      <c r="A168" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B168" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C168" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D168" s="11"/>
       <c r="E168" s="11"/>
       <c r="F168" s="11"/>
@@ -12368,7 +12595,9 @@
       <c r="Y168" s="11"/>
       <c r="Z168" s="11"/>
       <c r="AA168" s="11"/>
-      <c r="AB168" s="11"/>
+      <c r="AB168" s="11" t="n">
+        <v>5</v>
+      </c>
       <c r="AC168" s="11"/>
       <c r="AD168" s="11"/>
       <c r="AE168" s="11"/>
@@ -12404,16 +12633,24 @@
       <c r="BI168" s="11"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="12"/>
-      <c r="B169" s="12"/>
-      <c r="C169" s="12"/>
+      <c r="A169" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B169" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C169" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D169" s="12"/>
       <c r="E169" s="12"/>
       <c r="F169" s="12"/>
       <c r="G169" s="12"/>
       <c r="H169" s="12"/>
       <c r="I169" s="12"/>
-      <c r="J169" s="12"/>
+      <c r="J169" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="K169" s="12"/>
       <c r="L169" s="12"/>
       <c r="M169" s="12"/>
@@ -12467,16 +12704,24 @@
       <c r="BI169" s="12"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="11"/>
-      <c r="B170" s="11"/>
-      <c r="C170" s="11"/>
+      <c r="A170" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B170" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C170" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D170" s="11"/>
       <c r="E170" s="11"/>
       <c r="F170" s="11"/>
       <c r="G170" s="11"/>
       <c r="H170" s="11"/>
       <c r="I170" s="11"/>
-      <c r="J170" s="11"/>
+      <c r="J170" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="K170" s="11"/>
       <c r="L170" s="11"/>
       <c r="M170" s="11"/>
@@ -12520,7 +12765,9 @@
       <c r="AY170" s="11"/>
       <c r="AZ170" s="11"/>
       <c r="BA170" s="11"/>
-      <c r="BB170" s="11"/>
+      <c r="BB170" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="BC170" s="11"/>
       <c r="BD170" s="11"/>
       <c r="BE170" s="11"/>
@@ -12530,9 +12777,15 @@
       <c r="BI170" s="11"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="12"/>
-      <c r="B171" s="12"/>
-      <c r="C171" s="12"/>
+      <c r="A171" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B171" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C171" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D171" s="12"/>
       <c r="E171" s="12"/>
       <c r="F171" s="12"/>
@@ -12551,7 +12804,9 @@
       <c r="S171" s="12"/>
       <c r="T171" s="12"/>
       <c r="U171" s="12"/>
-      <c r="V171" s="12"/>
+      <c r="V171" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="W171" s="12"/>
       <c r="X171" s="12"/>
       <c r="Y171" s="12"/>
@@ -12593,9 +12848,15 @@
       <c r="BI171" s="12"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="11"/>
-      <c r="B172" s="11"/>
-      <c r="C172" s="11"/>
+      <c r="A172" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B172" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C172" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D172" s="11"/>
       <c r="E172" s="11"/>
       <c r="F172" s="11"/>
@@ -12625,7 +12886,9 @@
       <c r="AD172" s="11"/>
       <c r="AE172" s="11"/>
       <c r="AF172" s="11"/>
-      <c r="AG172" s="11"/>
+      <c r="AG172" s="11" t="n">
+        <v>370</v>
+      </c>
       <c r="AH172" s="11"/>
       <c r="AI172" s="11"/>
       <c r="AJ172" s="11"/>
@@ -12656,9 +12919,15 @@
       <c r="BI172" s="11"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="12"/>
-      <c r="B173" s="12"/>
-      <c r="C173" s="12"/>
+      <c r="A173" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B173" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C173" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D173" s="12"/>
       <c r="E173" s="12"/>
       <c r="F173" s="12"/>
@@ -12678,7 +12947,9 @@
       <c r="T173" s="12"/>
       <c r="U173" s="12"/>
       <c r="V173" s="12"/>
-      <c r="W173" s="12"/>
+      <c r="W173" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="X173" s="12"/>
       <c r="Y173" s="12"/>
       <c r="Z173" s="12"/>
@@ -12719,9 +12990,15 @@
       <c r="BI173" s="12"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="11"/>
-      <c r="B174" s="11"/>
-      <c r="C174" s="11"/>
+      <c r="A174" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B174" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C174" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D174" s="11"/>
       <c r="E174" s="11"/>
       <c r="F174" s="11"/>
@@ -12740,7 +13017,9 @@
       <c r="S174" s="11"/>
       <c r="T174" s="11"/>
       <c r="U174" s="11"/>
-      <c r="V174" s="11"/>
+      <c r="V174" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="W174" s="11"/>
       <c r="X174" s="11"/>
       <c r="Y174" s="11"/>
@@ -12782,9 +13061,15 @@
       <c r="BI174" s="11"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="12"/>
-      <c r="B175" s="12"/>
-      <c r="C175" s="12"/>
+      <c r="A175" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B175" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C175" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D175" s="12"/>
       <c r="E175" s="12"/>
       <c r="F175" s="12"/>
@@ -12809,7 +13094,9 @@
       <c r="Y175" s="12"/>
       <c r="Z175" s="12"/>
       <c r="AA175" s="12"/>
-      <c r="AB175" s="12"/>
+      <c r="AB175" s="12" t="n">
+        <v>5</v>
+      </c>
       <c r="AC175" s="12"/>
       <c r="AD175" s="12"/>
       <c r="AE175" s="12"/>
@@ -12845,7 +13132,9 @@
       <c r="BI175" s="12"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="11"/>
+      <c r="A176" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B176" s="11"/>
       <c r="C176" s="11"/>
       <c r="D176" s="11"/>
@@ -12908,7 +13197,9 @@
       <c r="BI176" s="11"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="12"/>
+      <c r="A177" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B177" s="12"/>
       <c r="C177" s="12"/>
       <c r="D177" s="12"/>
@@ -12971,7 +13262,9 @@
       <c r="BI177" s="12"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="11"/>
+      <c r="A178" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B178" s="11"/>
       <c r="C178" s="11"/>
       <c r="D178" s="11"/>
@@ -13034,7 +13327,9 @@
       <c r="BI178" s="11"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="12"/>
+      <c r="A179" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B179" s="12"/>
       <c r="C179" s="12"/>
       <c r="D179" s="12"/>
@@ -13097,7 +13392,9 @@
       <c r="BI179" s="12"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="11"/>
+      <c r="A180" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B180" s="11"/>
       <c r="C180" s="11"/>
       <c r="D180" s="11"/>
@@ -13160,7 +13457,9 @@
       <c r="BI180" s="11"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="12"/>
+      <c r="A181" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B181" s="12"/>
       <c r="C181" s="12"/>
       <c r="D181" s="12"/>
@@ -13223,7 +13522,9 @@
       <c r="BI181" s="12"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="11"/>
+      <c r="A182" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B182" s="11"/>
       <c r="C182" s="11"/>
       <c r="D182" s="11"/>
@@ -13286,7 +13587,9 @@
       <c r="BI182" s="11"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="12"/>
+      <c r="A183" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B183" s="12"/>
       <c r="C183" s="12"/>
       <c r="D183" s="12"/>
@@ -13349,7 +13652,9 @@
       <c r="BI183" s="12"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="11"/>
+      <c r="A184" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B184" s="11"/>
       <c r="C184" s="11"/>
       <c r="D184" s="11"/>
@@ -13412,7 +13717,9 @@
       <c r="BI184" s="11"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="12"/>
+      <c r="A185" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B185" s="12"/>
       <c r="C185" s="12"/>
       <c r="D185" s="12"/>
@@ -13475,7 +13782,9 @@
       <c r="BI185" s="12"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="11"/>
+      <c r="A186" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B186" s="11"/>
       <c r="C186" s="11"/>
       <c r="D186" s="11"/>
@@ -13538,7 +13847,9 @@
       <c r="BI186" s="11"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="12"/>
+      <c r="A187" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B187" s="12"/>
       <c r="C187" s="12"/>
       <c r="D187" s="12"/>
@@ -13601,7 +13912,9 @@
       <c r="BI187" s="12"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="11"/>
+      <c r="A188" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B188" s="11"/>
       <c r="C188" s="11"/>
       <c r="D188" s="11"/>
@@ -13664,7 +13977,9 @@
       <c r="BI188" s="11"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="12"/>
+      <c r="A189" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B189" s="12"/>
       <c r="C189" s="12"/>
       <c r="D189" s="12"/>
@@ -13727,7 +14042,9 @@
       <c r="BI189" s="12"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="11"/>
+      <c r="A190" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B190" s="11"/>
       <c r="C190" s="11"/>
       <c r="D190" s="11"/>
@@ -13790,7 +14107,9 @@
       <c r="BI190" s="11"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="12"/>
+      <c r="A191" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B191" s="12"/>
       <c r="C191" s="12"/>
       <c r="D191" s="12"/>
@@ -13853,7 +14172,9 @@
       <c r="BI191" s="12"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="11"/>
+      <c r="A192" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B192" s="11"/>
       <c r="C192" s="11"/>
       <c r="D192" s="11"/>
@@ -13916,7 +14237,9 @@
       <c r="BI192" s="11"/>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="12"/>
+      <c r="A193" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B193" s="12"/>
       <c r="C193" s="12"/>
       <c r="D193" s="12"/>
@@ -13979,7 +14302,9 @@
       <c r="BI193" s="12"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="11"/>
+      <c r="A194" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B194" s="11"/>
       <c r="C194" s="11"/>
       <c r="D194" s="11"/>
@@ -14042,7 +14367,9 @@
       <c r="BI194" s="11"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="12"/>
+      <c r="A195" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B195" s="12"/>
       <c r="C195" s="12"/>
       <c r="D195" s="12"/>
@@ -14105,7 +14432,9 @@
       <c r="BI195" s="12"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="11"/>
+      <c r="A196" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B196" s="11"/>
       <c r="C196" s="11"/>
       <c r="D196" s="11"/>
@@ -14168,7 +14497,9 @@
       <c r="BI196" s="11"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="12"/>
+      <c r="A197" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B197" s="12"/>
       <c r="C197" s="12"/>
       <c r="D197" s="12"/>
@@ -14231,7 +14562,9 @@
       <c r="BI197" s="12"/>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="11"/>
+      <c r="A198" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B198" s="11"/>
       <c r="C198" s="11"/>
       <c r="D198" s="11"/>
@@ -14294,7 +14627,9 @@
       <c r="BI198" s="11"/>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="12"/>
+      <c r="A199" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B199" s="12"/>
       <c r="C199" s="12"/>
       <c r="D199" s="12"/>
@@ -14357,7 +14692,9 @@
       <c r="BI199" s="12"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="11"/>
+      <c r="A200" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B200" s="11"/>
       <c r="C200" s="11"/>
       <c r="D200" s="11"/>
@@ -14420,7 +14757,9 @@
       <c r="BI200" s="11"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="12"/>
+      <c r="A201" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B201" s="12"/>
       <c r="C201" s="12"/>
       <c r="D201" s="12"/>
@@ -14483,7 +14822,9 @@
       <c r="BI201" s="12"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="11"/>
+      <c r="A202" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B202" s="11"/>
       <c r="C202" s="11"/>
       <c r="D202" s="11"/>
@@ -14546,7 +14887,9 @@
       <c r="BI202" s="11"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="12"/>
+      <c r="A203" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B203" s="12"/>
       <c r="C203" s="12"/>
       <c r="D203" s="12"/>
@@ -14609,7 +14952,9 @@
       <c r="BI203" s="12"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="11"/>
+      <c r="A204" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B204" s="11"/>
       <c r="C204" s="11"/>
       <c r="D204" s="11"/>

</xml_diff>

<commit_message>
Up to 200 drops
</commit_message>
<xml_diff>
--- a/Drops.xlsx
+++ b/Drops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="67">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t xml:space="preserve">2020/3/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/3/25</t>
   </si>
 </sst>
 </file>
@@ -494,8 +497,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ393"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B175" activeCellId="0" sqref="B175"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D198" activeCellId="0" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13133,10 +13136,14 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B176" s="11"/>
-      <c r="C176" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B176" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C176" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D176" s="11"/>
       <c r="E176" s="11"/>
       <c r="F176" s="11"/>
@@ -13166,7 +13173,9 @@
       <c r="AD176" s="11"/>
       <c r="AE176" s="11"/>
       <c r="AF176" s="11"/>
-      <c r="AG176" s="11"/>
+      <c r="AG176" s="11" t="n">
+        <v>370</v>
+      </c>
       <c r="AH176" s="11"/>
       <c r="AI176" s="11"/>
       <c r="AJ176" s="11"/>
@@ -13198,10 +13207,14 @@
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B177" s="12"/>
-      <c r="C177" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B177" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C177" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D177" s="12"/>
       <c r="E177" s="12"/>
       <c r="F177" s="12"/>
@@ -13226,7 +13239,9 @@
       <c r="Y177" s="12"/>
       <c r="Z177" s="12"/>
       <c r="AA177" s="12"/>
-      <c r="AB177" s="12"/>
+      <c r="AB177" s="12" t="n">
+        <v>5</v>
+      </c>
       <c r="AC177" s="12"/>
       <c r="AD177" s="12"/>
       <c r="AE177" s="12"/>
@@ -13263,10 +13278,14 @@
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B178" s="11"/>
-      <c r="C178" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B178" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C178" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D178" s="11"/>
       <c r="E178" s="11"/>
       <c r="F178" s="11"/>
@@ -13291,7 +13310,9 @@
       <c r="Y178" s="11"/>
       <c r="Z178" s="11"/>
       <c r="AA178" s="11"/>
-      <c r="AB178" s="11"/>
+      <c r="AB178" s="11" t="n">
+        <v>5</v>
+      </c>
       <c r="AC178" s="11"/>
       <c r="AD178" s="11"/>
       <c r="AE178" s="11"/>
@@ -13328,17 +13349,23 @@
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B179" s="12"/>
-      <c r="C179" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B179" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C179" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D179" s="12"/>
       <c r="E179" s="12"/>
       <c r="F179" s="12"/>
       <c r="G179" s="12"/>
       <c r="H179" s="12"/>
       <c r="I179" s="12"/>
-      <c r="J179" s="12"/>
+      <c r="J179" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="K179" s="12"/>
       <c r="L179" s="12"/>
       <c r="M179" s="12"/>
@@ -13393,10 +13420,14 @@
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B180" s="11"/>
-      <c r="C180" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B180" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C180" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D180" s="11"/>
       <c r="E180" s="11"/>
       <c r="F180" s="11"/>
@@ -13404,7 +13435,9 @@
       <c r="H180" s="11"/>
       <c r="I180" s="11"/>
       <c r="J180" s="11"/>
-      <c r="K180" s="11"/>
+      <c r="K180" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="L180" s="11"/>
       <c r="M180" s="11"/>
       <c r="N180" s="11"/>
@@ -13458,17 +13491,23 @@
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B181" s="12"/>
-      <c r="C181" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B181" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C181" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D181" s="12"/>
       <c r="E181" s="12"/>
       <c r="F181" s="12"/>
       <c r="G181" s="12"/>
       <c r="H181" s="12"/>
       <c r="I181" s="12"/>
-      <c r="J181" s="12"/>
+      <c r="J181" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="K181" s="12"/>
       <c r="L181" s="12"/>
       <c r="M181" s="12"/>
@@ -13523,10 +13562,14 @@
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B182" s="11"/>
-      <c r="C182" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B182" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C182" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D182" s="11"/>
       <c r="E182" s="11"/>
       <c r="F182" s="11"/>
@@ -13556,7 +13599,9 @@
       <c r="AD182" s="11"/>
       <c r="AE182" s="11"/>
       <c r="AF182" s="11"/>
-      <c r="AG182" s="11"/>
+      <c r="AG182" s="11" t="n">
+        <v>771</v>
+      </c>
       <c r="AH182" s="11"/>
       <c r="AI182" s="11"/>
       <c r="AJ182" s="11"/>
@@ -13588,10 +13633,14 @@
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B183" s="12"/>
-      <c r="C183" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B183" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C183" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D183" s="12"/>
       <c r="E183" s="12"/>
       <c r="F183" s="12"/>
@@ -13613,7 +13662,9 @@
       <c r="V183" s="12"/>
       <c r="W183" s="12"/>
       <c r="X183" s="12"/>
-      <c r="Y183" s="12"/>
+      <c r="Y183" s="12" t="n">
+        <v>75</v>
+      </c>
       <c r="Z183" s="12"/>
       <c r="AA183" s="12"/>
       <c r="AB183" s="12"/>
@@ -13653,10 +13704,14 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B184" s="11"/>
-      <c r="C184" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B184" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C184" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D184" s="11"/>
       <c r="E184" s="11"/>
       <c r="F184" s="11"/>
@@ -13676,7 +13731,9 @@
       <c r="T184" s="11"/>
       <c r="U184" s="11"/>
       <c r="V184" s="11"/>
-      <c r="W184" s="11"/>
+      <c r="W184" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X184" s="11"/>
       <c r="Y184" s="11"/>
       <c r="Z184" s="11"/>
@@ -13718,10 +13775,14 @@
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B185" s="12"/>
-      <c r="C185" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B185" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C185" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D185" s="12"/>
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
@@ -13729,7 +13790,9 @@
       <c r="H185" s="12"/>
       <c r="I185" s="12"/>
       <c r="J185" s="12"/>
-      <c r="K185" s="12"/>
+      <c r="K185" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="L185" s="12"/>
       <c r="M185" s="12"/>
       <c r="N185" s="12"/>
@@ -13783,10 +13846,14 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B186" s="11"/>
-      <c r="C186" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B186" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C186" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D186" s="11"/>
       <c r="E186" s="11"/>
       <c r="F186" s="11"/>
@@ -13810,7 +13877,9 @@
       <c r="X186" s="11"/>
       <c r="Y186" s="11"/>
       <c r="Z186" s="11"/>
-      <c r="AA186" s="11"/>
+      <c r="AA186" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AB186" s="11"/>
       <c r="AC186" s="11"/>
       <c r="AD186" s="11"/>
@@ -13848,10 +13917,14 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B187" s="12"/>
-      <c r="C187" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B187" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C187" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D187" s="12"/>
       <c r="E187" s="12"/>
       <c r="F187" s="12"/>
@@ -13872,7 +13945,9 @@
       <c r="U187" s="12"/>
       <c r="V187" s="12"/>
       <c r="W187" s="12"/>
-      <c r="X187" s="12"/>
+      <c r="X187" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="Y187" s="12"/>
       <c r="Z187" s="12"/>
       <c r="AA187" s="12"/>
@@ -13913,10 +13988,14 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B188" s="11"/>
-      <c r="C188" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B188" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C188" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D188" s="11"/>
       <c r="E188" s="11"/>
       <c r="F188" s="11"/>
@@ -13947,7 +14026,9 @@
       <c r="AE188" s="11"/>
       <c r="AF188" s="11"/>
       <c r="AG188" s="11"/>
-      <c r="AH188" s="11"/>
+      <c r="AH188" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="AI188" s="11"/>
       <c r="AJ188" s="11"/>
       <c r="AK188" s="11"/>
@@ -13978,10 +14059,14 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B189" s="12"/>
-      <c r="C189" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B189" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C189" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D189" s="12"/>
       <c r="E189" s="12"/>
       <c r="F189" s="12"/>
@@ -14012,7 +14097,9 @@
       <c r="AE189" s="12"/>
       <c r="AF189" s="12"/>
       <c r="AG189" s="12"/>
-      <c r="AH189" s="12"/>
+      <c r="AH189" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="AI189" s="12"/>
       <c r="AJ189" s="12"/>
       <c r="AK189" s="12"/>
@@ -14043,10 +14130,14 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B190" s="11"/>
-      <c r="C190" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B190" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C190" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D190" s="11"/>
       <c r="E190" s="11"/>
       <c r="F190" s="11"/>
@@ -14065,7 +14156,9 @@
       <c r="S190" s="11"/>
       <c r="T190" s="11"/>
       <c r="U190" s="11"/>
-      <c r="V190" s="11"/>
+      <c r="V190" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="W190" s="11"/>
       <c r="X190" s="11"/>
       <c r="Y190" s="11"/>
@@ -14108,10 +14201,14 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B191" s="12"/>
-      <c r="C191" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B191" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C191" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D191" s="12"/>
       <c r="E191" s="12"/>
       <c r="F191" s="12"/>
@@ -14131,7 +14228,9 @@
       <c r="T191" s="12"/>
       <c r="U191" s="12"/>
       <c r="V191" s="12"/>
-      <c r="W191" s="12"/>
+      <c r="W191" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="X191" s="12"/>
       <c r="Y191" s="12"/>
       <c r="Z191" s="12"/>
@@ -14173,10 +14272,14 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B192" s="11"/>
-      <c r="C192" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B192" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C192" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D192" s="11"/>
       <c r="E192" s="11"/>
       <c r="F192" s="11"/>
@@ -14196,7 +14299,9 @@
       <c r="T192" s="11"/>
       <c r="U192" s="11"/>
       <c r="V192" s="11"/>
-      <c r="W192" s="11"/>
+      <c r="W192" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X192" s="11"/>
       <c r="Y192" s="11"/>
       <c r="Z192" s="11"/>
@@ -14238,17 +14343,23 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B193" s="12"/>
-      <c r="C193" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B193" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C193" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D193" s="12"/>
       <c r="E193" s="12"/>
       <c r="F193" s="12"/>
       <c r="G193" s="12"/>
       <c r="H193" s="12"/>
       <c r="I193" s="12"/>
-      <c r="J193" s="12"/>
+      <c r="J193" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="K193" s="12"/>
       <c r="L193" s="12"/>
       <c r="M193" s="12"/>
@@ -14303,10 +14414,14 @@
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B194" s="11"/>
-      <c r="C194" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B194" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C194" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D194" s="11"/>
       <c r="E194" s="11"/>
       <c r="F194" s="11"/>
@@ -14336,7 +14451,9 @@
       <c r="AD194" s="11"/>
       <c r="AE194" s="11"/>
       <c r="AF194" s="11"/>
-      <c r="AG194" s="11"/>
+      <c r="AG194" s="11" t="n">
+        <v>370</v>
+      </c>
       <c r="AH194" s="11"/>
       <c r="AI194" s="11"/>
       <c r="AJ194" s="11"/>
@@ -14368,10 +14485,14 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B195" s="12"/>
-      <c r="C195" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B195" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C195" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D195" s="12"/>
       <c r="E195" s="12"/>
       <c r="F195" s="12"/>
@@ -14399,7 +14520,9 @@
       <c r="AB195" s="12"/>
       <c r="AC195" s="12"/>
       <c r="AD195" s="12"/>
-      <c r="AE195" s="12"/>
+      <c r="AE195" s="12" t="n">
+        <v>40</v>
+      </c>
       <c r="AF195" s="12"/>
       <c r="AG195" s="12"/>
       <c r="AH195" s="12"/>
@@ -14433,10 +14556,14 @@
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B196" s="11"/>
-      <c r="C196" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B196" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C196" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D196" s="11"/>
       <c r="E196" s="11"/>
       <c r="F196" s="11"/>
@@ -14457,7 +14584,9 @@
       <c r="U196" s="11"/>
       <c r="V196" s="11"/>
       <c r="W196" s="11"/>
-      <c r="X196" s="11"/>
+      <c r="X196" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="Y196" s="11"/>
       <c r="Z196" s="11"/>
       <c r="AA196" s="11"/>
@@ -14498,10 +14627,14 @@
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B197" s="12"/>
-      <c r="C197" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B197" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C197" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D197" s="12"/>
       <c r="E197" s="12"/>
       <c r="F197" s="12"/>
@@ -14509,7 +14642,9 @@
       <c r="H197" s="12"/>
       <c r="I197" s="12"/>
       <c r="J197" s="12"/>
-      <c r="K197" s="12"/>
+      <c r="K197" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="L197" s="12"/>
       <c r="M197" s="12"/>
       <c r="N197" s="12"/>
@@ -14563,10 +14698,14 @@
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B198" s="11"/>
-      <c r="C198" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B198" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C198" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D198" s="11"/>
       <c r="E198" s="11"/>
       <c r="F198" s="11"/>
@@ -14574,7 +14713,9 @@
       <c r="H198" s="11"/>
       <c r="I198" s="11"/>
       <c r="J198" s="11"/>
-      <c r="K198" s="11"/>
+      <c r="K198" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="L198" s="11"/>
       <c r="M198" s="11"/>
       <c r="N198" s="11"/>
@@ -14628,10 +14769,14 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B199" s="12"/>
-      <c r="C199" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B199" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C199" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D199" s="12"/>
       <c r="E199" s="12"/>
       <c r="F199" s="12"/>
@@ -14650,7 +14795,9 @@
       <c r="S199" s="12"/>
       <c r="T199" s="12"/>
       <c r="U199" s="12"/>
-      <c r="V199" s="12"/>
+      <c r="V199" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="W199" s="12"/>
       <c r="X199" s="12"/>
       <c r="Y199" s="12"/>
@@ -14693,10 +14840,14 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B200" s="11"/>
-      <c r="C200" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B200" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C200" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D200" s="11"/>
       <c r="E200" s="11"/>
       <c r="F200" s="11"/>
@@ -14730,7 +14881,9 @@
       <c r="AH200" s="11"/>
       <c r="AI200" s="11"/>
       <c r="AJ200" s="11"/>
-      <c r="AK200" s="11"/>
+      <c r="AK200" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="AL200" s="11"/>
       <c r="AM200" s="11"/>
       <c r="AN200" s="11"/>
@@ -14758,10 +14911,14 @@
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B201" s="12"/>
-      <c r="C201" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B201" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C201" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D201" s="12"/>
       <c r="E201" s="12"/>
       <c r="F201" s="12"/>
@@ -14807,7 +14964,9 @@
       <c r="AT201" s="12"/>
       <c r="AU201" s="12"/>
       <c r="AV201" s="12"/>
-      <c r="AW201" s="12"/>
+      <c r="AW201" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="AX201" s="12"/>
       <c r="AY201" s="12"/>
       <c r="AZ201" s="12"/>
@@ -14823,10 +14982,14 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B202" s="11"/>
-      <c r="C202" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B202" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C202" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D202" s="11"/>
       <c r="E202" s="11"/>
       <c r="F202" s="11"/>
@@ -14838,7 +15001,9 @@
       <c r="L202" s="11"/>
       <c r="M202" s="11"/>
       <c r="N202" s="11"/>
-      <c r="O202" s="11"/>
+      <c r="O202" s="11" t="n">
+        <v>25</v>
+      </c>
       <c r="P202" s="11"/>
       <c r="Q202" s="11"/>
       <c r="R202" s="11"/>
@@ -14888,15 +15053,21 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B203" s="12"/>
-      <c r="C203" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B203" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C203" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D203" s="12"/>
       <c r="E203" s="12"/>
       <c r="F203" s="12"/>
       <c r="G203" s="12"/>
-      <c r="H203" s="12"/>
+      <c r="H203" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="I203" s="12"/>
       <c r="J203" s="12"/>
       <c r="K203" s="12"/>
@@ -14952,9 +15123,7 @@
       <c r="BI203" s="12"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="11" t="s">
-        <v>65</v>
-      </c>
+      <c r="A204" s="11"/>
       <c r="B204" s="11"/>
       <c r="C204" s="11"/>
       <c r="D204" s="11"/>

</xml_diff>

<commit_message>
Past the 300th mark
</commit_message>
<xml_diff>
--- a/Drops.xlsx
+++ b/Drops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="69">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">2020/3/26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/3/27</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
   <dimension ref="A1:AMJ393"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A225" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C289" activeCellId="0" sqref="C289"/>
+      <selection pane="topLeft" activeCell="C303" activeCellId="0" sqref="C303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19030,10 +19033,14 @@
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B259" s="12"/>
-      <c r="C259" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="B259" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C259" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D259" s="12"/>
       <c r="E259" s="12"/>
       <c r="F259" s="12"/>
@@ -19053,7 +19060,9 @@
       <c r="T259" s="12"/>
       <c r="U259" s="12"/>
       <c r="V259" s="12"/>
-      <c r="W259" s="12"/>
+      <c r="W259" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="X259" s="12"/>
       <c r="Y259" s="12"/>
       <c r="Z259" s="12"/>
@@ -19095,15 +19104,21 @@
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B260" s="11"/>
-      <c r="C260" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="B260" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C260" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D260" s="11"/>
       <c r="E260" s="11"/>
       <c r="F260" s="11"/>
       <c r="G260" s="11"/>
-      <c r="H260" s="11"/>
+      <c r="H260" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="I260" s="11"/>
       <c r="J260" s="11"/>
       <c r="K260" s="11"/>
@@ -19160,15 +19175,21 @@
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B261" s="12"/>
-      <c r="C261" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="B261" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C261" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D261" s="12"/>
       <c r="E261" s="12"/>
       <c r="F261" s="12"/>
       <c r="G261" s="12"/>
-      <c r="H261" s="12"/>
+      <c r="H261" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="I261" s="12"/>
       <c r="J261" s="12"/>
       <c r="K261" s="12"/>
@@ -19225,10 +19246,14 @@
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B262" s="11"/>
-      <c r="C262" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="B262" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C262" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D262" s="11"/>
       <c r="E262" s="11"/>
       <c r="F262" s="11"/>
@@ -19252,7 +19277,9 @@
       <c r="X262" s="11"/>
       <c r="Y262" s="11"/>
       <c r="Z262" s="11"/>
-      <c r="AA262" s="11"/>
+      <c r="AA262" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AB262" s="11"/>
       <c r="AC262" s="11"/>
       <c r="AD262" s="11"/>
@@ -19290,10 +19317,14 @@
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B263" s="12"/>
-      <c r="C263" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="B263" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C263" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D263" s="12"/>
       <c r="E263" s="12"/>
       <c r="F263" s="12"/>
@@ -19306,7 +19337,9 @@
       <c r="M263" s="12"/>
       <c r="N263" s="12"/>
       <c r="O263" s="12"/>
-      <c r="P263" s="12"/>
+      <c r="P263" s="12" t="n">
+        <v>30</v>
+      </c>
       <c r="Q263" s="12"/>
       <c r="R263" s="12"/>
       <c r="S263" s="12"/>
@@ -19355,10 +19388,14 @@
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B264" s="11"/>
-      <c r="C264" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="B264" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C264" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D264" s="11"/>
       <c r="E264" s="11"/>
       <c r="F264" s="11"/>
@@ -19393,7 +19430,9 @@
       <c r="AI264" s="11"/>
       <c r="AJ264" s="11"/>
       <c r="AK264" s="11"/>
-      <c r="AL264" s="11"/>
+      <c r="AL264" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="AM264" s="11"/>
       <c r="AN264" s="11"/>
       <c r="AO264" s="11"/>
@@ -19420,10 +19459,14 @@
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B265" s="12"/>
-      <c r="C265" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="B265" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C265" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D265" s="12"/>
       <c r="E265" s="12"/>
       <c r="F265" s="12"/>
@@ -19448,7 +19491,9 @@
       <c r="Y265" s="12"/>
       <c r="Z265" s="12"/>
       <c r="AA265" s="12"/>
-      <c r="AB265" s="12"/>
+      <c r="AB265" s="12" t="n">
+        <v>5</v>
+      </c>
       <c r="AC265" s="12"/>
       <c r="AD265" s="12"/>
       <c r="AE265" s="12"/>
@@ -19485,10 +19530,14 @@
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B266" s="11"/>
-      <c r="C266" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="B266" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C266" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D266" s="11"/>
       <c r="E266" s="11"/>
       <c r="F266" s="11"/>
@@ -19508,7 +19557,9 @@
       <c r="T266" s="11"/>
       <c r="U266" s="11"/>
       <c r="V266" s="11"/>
-      <c r="W266" s="11"/>
+      <c r="W266" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="X266" s="11"/>
       <c r="Y266" s="11"/>
       <c r="Z266" s="11"/>
@@ -19550,10 +19601,14 @@
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B267" s="12"/>
-      <c r="C267" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="B267" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C267" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D267" s="12"/>
       <c r="E267" s="12"/>
       <c r="F267" s="12"/>
@@ -19562,7 +19617,9 @@
       <c r="I267" s="12"/>
       <c r="J267" s="12"/>
       <c r="K267" s="12"/>
-      <c r="L267" s="12"/>
+      <c r="L267" s="12" t="n">
+        <v>20</v>
+      </c>
       <c r="M267" s="12"/>
       <c r="N267" s="12"/>
       <c r="O267" s="12"/>
@@ -19614,9 +19671,15 @@
       <c r="BI267" s="12"/>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="11"/>
-      <c r="B268" s="11"/>
-      <c r="C268" s="11"/>
+      <c r="A268" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B268" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C268" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D268" s="11"/>
       <c r="E268" s="11"/>
       <c r="F268" s="11"/>
@@ -19624,7 +19687,9 @@
       <c r="H268" s="11"/>
       <c r="I268" s="11"/>
       <c r="J268" s="11"/>
-      <c r="K268" s="11"/>
+      <c r="K268" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="L268" s="11"/>
       <c r="M268" s="11"/>
       <c r="N268" s="11"/>
@@ -19677,9 +19742,15 @@
       <c r="BI268" s="11"/>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="12"/>
-      <c r="B269" s="12"/>
-      <c r="C269" s="12"/>
+      <c r="A269" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B269" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C269" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D269" s="12"/>
       <c r="E269" s="12"/>
       <c r="F269" s="12"/>
@@ -19689,7 +19760,9 @@
       <c r="J269" s="12"/>
       <c r="K269" s="12"/>
       <c r="L269" s="12"/>
-      <c r="M269" s="12"/>
+      <c r="M269" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="N269" s="12"/>
       <c r="O269" s="12"/>
       <c r="P269" s="12"/>
@@ -19740,9 +19813,15 @@
       <c r="BI269" s="12"/>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="11"/>
-      <c r="B270" s="11"/>
-      <c r="C270" s="11"/>
+      <c r="A270" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B270" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C270" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D270" s="11"/>
       <c r="E270" s="11"/>
       <c r="F270" s="11"/>
@@ -19753,7 +19832,9 @@
       <c r="K270" s="11"/>
       <c r="L270" s="11"/>
       <c r="M270" s="11"/>
-      <c r="N270" s="11"/>
+      <c r="N270" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="O270" s="11"/>
       <c r="P270" s="11"/>
       <c r="Q270" s="11"/>
@@ -19803,9 +19884,15 @@
       <c r="BI270" s="11"/>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="12"/>
-      <c r="B271" s="12"/>
-      <c r="C271" s="12"/>
+      <c r="A271" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B271" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C271" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D271" s="12"/>
       <c r="E271" s="12"/>
       <c r="F271" s="12"/>
@@ -19835,7 +19922,9 @@
       <c r="AD271" s="12"/>
       <c r="AE271" s="12"/>
       <c r="AF271" s="12"/>
-      <c r="AG271" s="12"/>
+      <c r="AG271" s="12" t="n">
+        <v>766</v>
+      </c>
       <c r="AH271" s="12"/>
       <c r="AI271" s="12"/>
       <c r="AJ271" s="12"/>
@@ -19856,7 +19945,9 @@
       <c r="AY271" s="12"/>
       <c r="AZ271" s="12"/>
       <c r="BA271" s="12"/>
-      <c r="BB271" s="12"/>
+      <c r="BB271" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="BC271" s="12"/>
       <c r="BD271" s="12"/>
       <c r="BE271" s="12"/>
@@ -19866,14 +19957,22 @@
       <c r="BI271" s="12"/>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="11"/>
-      <c r="B272" s="11"/>
-      <c r="C272" s="11"/>
+      <c r="A272" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B272" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C272" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D272" s="11"/>
       <c r="E272" s="11"/>
       <c r="F272" s="11"/>
       <c r="G272" s="11"/>
-      <c r="H272" s="11"/>
+      <c r="H272" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="I272" s="11"/>
       <c r="J272" s="11"/>
       <c r="K272" s="11"/>
@@ -19929,9 +20028,15 @@
       <c r="BI272" s="11"/>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="12"/>
-      <c r="B273" s="12"/>
-      <c r="C273" s="12"/>
+      <c r="A273" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B273" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C273" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D273" s="12"/>
       <c r="E273" s="12"/>
       <c r="F273" s="12"/>
@@ -19992,14 +20097,22 @@
       <c r="BI273" s="12"/>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="11"/>
-      <c r="B274" s="11"/>
-      <c r="C274" s="11"/>
+      <c r="A274" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B274" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C274" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D274" s="11"/>
       <c r="E274" s="11"/>
       <c r="F274" s="11"/>
       <c r="G274" s="11"/>
-      <c r="H274" s="11"/>
+      <c r="H274" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="I274" s="11"/>
       <c r="J274" s="11"/>
       <c r="K274" s="11"/>
@@ -20055,14 +20168,22 @@
       <c r="BI274" s="11"/>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="12"/>
-      <c r="B275" s="12"/>
-      <c r="C275" s="12"/>
+      <c r="A275" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B275" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C275" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D275" s="12"/>
       <c r="E275" s="12"/>
       <c r="F275" s="12"/>
       <c r="G275" s="12"/>
-      <c r="H275" s="12"/>
+      <c r="H275" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="I275" s="12"/>
       <c r="J275" s="12"/>
       <c r="K275" s="12"/>
@@ -20118,9 +20239,15 @@
       <c r="BI275" s="12"/>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="11"/>
-      <c r="B276" s="11"/>
-      <c r="C276" s="11"/>
+      <c r="A276" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B276" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C276" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D276" s="11"/>
       <c r="E276" s="11"/>
       <c r="F276" s="11"/>
@@ -20141,7 +20268,9 @@
       <c r="U276" s="11"/>
       <c r="V276" s="11"/>
       <c r="W276" s="11"/>
-      <c r="X276" s="11"/>
+      <c r="X276" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="Y276" s="11"/>
       <c r="Z276" s="11"/>
       <c r="AA276" s="11"/>
@@ -20181,9 +20310,15 @@
       <c r="BI276" s="11"/>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="12"/>
-      <c r="B277" s="12"/>
-      <c r="C277" s="12"/>
+      <c r="A277" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B277" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C277" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D277" s="12"/>
       <c r="E277" s="12"/>
       <c r="F277" s="12"/>
@@ -20206,7 +20341,9 @@
       <c r="W277" s="12"/>
       <c r="X277" s="12"/>
       <c r="Y277" s="12"/>
-      <c r="Z277" s="12"/>
+      <c r="Z277" s="12" t="n">
+        <v>75</v>
+      </c>
       <c r="AA277" s="12"/>
       <c r="AB277" s="12"/>
       <c r="AC277" s="12"/>
@@ -20244,9 +20381,15 @@
       <c r="BI277" s="12"/>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="11"/>
-      <c r="B278" s="11"/>
-      <c r="C278" s="11"/>
+      <c r="A278" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B278" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C278" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D278" s="11"/>
       <c r="E278" s="11"/>
       <c r="F278" s="11"/>
@@ -20259,7 +20402,9 @@
       <c r="M278" s="11"/>
       <c r="N278" s="11"/>
       <c r="O278" s="11"/>
-      <c r="P278" s="11"/>
+      <c r="P278" s="11" t="n">
+        <v>30</v>
+      </c>
       <c r="Q278" s="11"/>
       <c r="R278" s="11"/>
       <c r="S278" s="11"/>
@@ -20307,9 +20452,15 @@
       <c r="BI278" s="11"/>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="12"/>
-      <c r="B279" s="12"/>
-      <c r="C279" s="12"/>
+      <c r="A279" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B279" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C279" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D279" s="12"/>
       <c r="E279" s="12"/>
       <c r="F279" s="12"/>
@@ -20322,7 +20473,9 @@
       <c r="M279" s="12"/>
       <c r="N279" s="12"/>
       <c r="O279" s="12"/>
-      <c r="P279" s="12"/>
+      <c r="P279" s="12" t="n">
+        <v>30</v>
+      </c>
       <c r="Q279" s="12"/>
       <c r="R279" s="12"/>
       <c r="S279" s="12"/>
@@ -20370,9 +20523,15 @@
       <c r="BI279" s="12"/>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="11"/>
-      <c r="B280" s="11"/>
-      <c r="C280" s="11"/>
+      <c r="A280" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B280" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C280" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D280" s="11"/>
       <c r="E280" s="11"/>
       <c r="F280" s="11"/>
@@ -20395,7 +20554,9 @@
       <c r="W280" s="11"/>
       <c r="X280" s="11"/>
       <c r="Y280" s="11"/>
-      <c r="Z280" s="11"/>
+      <c r="Z280" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AA280" s="11"/>
       <c r="AB280" s="11"/>
       <c r="AC280" s="11"/>
@@ -20433,9 +20594,15 @@
       <c r="BI280" s="11"/>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="12"/>
-      <c r="B281" s="12"/>
-      <c r="C281" s="12"/>
+      <c r="A281" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B281" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C281" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D281" s="12"/>
       <c r="E281" s="12"/>
       <c r="F281" s="12"/>
@@ -20465,7 +20632,9 @@
       <c r="AD281" s="12"/>
       <c r="AE281" s="12"/>
       <c r="AF281" s="12"/>
-      <c r="AG281" s="12"/>
+      <c r="AG281" s="12" t="n">
+        <v>370</v>
+      </c>
       <c r="AH281" s="12"/>
       <c r="AI281" s="12"/>
       <c r="AJ281" s="12"/>
@@ -20496,9 +20665,15 @@
       <c r="BI281" s="12"/>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="11"/>
-      <c r="B282" s="11"/>
-      <c r="C282" s="11"/>
+      <c r="A282" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B282" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C282" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D282" s="11"/>
       <c r="E282" s="11"/>
       <c r="F282" s="11"/>
@@ -20522,7 +20697,9 @@
       <c r="X282" s="11"/>
       <c r="Y282" s="11"/>
       <c r="Z282" s="11"/>
-      <c r="AA282" s="11"/>
+      <c r="AA282" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AB282" s="11"/>
       <c r="AC282" s="11"/>
       <c r="AD282" s="11"/>
@@ -20559,9 +20736,15 @@
       <c r="BI282" s="11"/>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="12"/>
-      <c r="B283" s="12"/>
-      <c r="C283" s="12"/>
+      <c r="A283" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B283" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C283" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D283" s="12"/>
       <c r="E283" s="12"/>
       <c r="F283" s="12"/>
@@ -20570,7 +20753,9 @@
       <c r="I283" s="12"/>
       <c r="J283" s="12"/>
       <c r="K283" s="12"/>
-      <c r="L283" s="12"/>
+      <c r="L283" s="12" t="n">
+        <v>20</v>
+      </c>
       <c r="M283" s="12"/>
       <c r="N283" s="12"/>
       <c r="O283" s="12"/>
@@ -20622,11 +20807,19 @@
       <c r="BI283" s="12"/>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="11"/>
-      <c r="B284" s="11"/>
-      <c r="C284" s="11"/>
+      <c r="A284" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B284" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C284" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D284" s="11"/>
-      <c r="E284" s="11"/>
+      <c r="E284" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="F284" s="11"/>
       <c r="G284" s="11"/>
       <c r="H284" s="11"/>
@@ -20685,9 +20878,15 @@
       <c r="BI284" s="11"/>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="12"/>
-      <c r="B285" s="12"/>
-      <c r="C285" s="12"/>
+      <c r="A285" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B285" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C285" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D285" s="12"/>
       <c r="E285" s="12"/>
       <c r="F285" s="12"/>
@@ -20717,7 +20916,9 @@
       <c r="AD285" s="12"/>
       <c r="AE285" s="12"/>
       <c r="AF285" s="12"/>
-      <c r="AG285" s="12"/>
+      <c r="AG285" s="12" t="n">
+        <v>370</v>
+      </c>
       <c r="AH285" s="12"/>
       <c r="AI285" s="12"/>
       <c r="AJ285" s="12"/>
@@ -20738,7 +20939,9 @@
       <c r="AY285" s="12"/>
       <c r="AZ285" s="12"/>
       <c r="BA285" s="12"/>
-      <c r="BB285" s="12"/>
+      <c r="BB285" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="BC285" s="12"/>
       <c r="BD285" s="12"/>
       <c r="BE285" s="12"/>
@@ -20748,9 +20951,15 @@
       <c r="BI285" s="12"/>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="11"/>
-      <c r="B286" s="11"/>
-      <c r="C286" s="11"/>
+      <c r="A286" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B286" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C286" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D286" s="11"/>
       <c r="E286" s="11"/>
       <c r="F286" s="11"/>
@@ -20774,7 +20983,9 @@
       <c r="X286" s="11"/>
       <c r="Y286" s="11"/>
       <c r="Z286" s="11"/>
-      <c r="AA286" s="11"/>
+      <c r="AA286" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AB286" s="11"/>
       <c r="AC286" s="11"/>
       <c r="AD286" s="11"/>
@@ -20811,9 +21022,15 @@
       <c r="BI286" s="11"/>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="12"/>
-      <c r="B287" s="12"/>
-      <c r="C287" s="12"/>
+      <c r="A287" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B287" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C287" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D287" s="12"/>
       <c r="E287" s="12"/>
       <c r="F287" s="12"/>
@@ -20833,7 +21050,9 @@
       <c r="T287" s="12"/>
       <c r="U287" s="12"/>
       <c r="V287" s="12"/>
-      <c r="W287" s="12"/>
+      <c r="W287" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="X287" s="12"/>
       <c r="Y287" s="12"/>
       <c r="Z287" s="12"/>
@@ -20874,9 +21093,15 @@
       <c r="BI287" s="12"/>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="11"/>
-      <c r="B288" s="11"/>
-      <c r="C288" s="11"/>
+      <c r="A288" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B288" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C288" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D288" s="11"/>
       <c r="E288" s="11"/>
       <c r="F288" s="11"/>
@@ -20904,7 +21129,9 @@
       <c r="AB288" s="11"/>
       <c r="AC288" s="11"/>
       <c r="AD288" s="11"/>
-      <c r="AE288" s="11"/>
+      <c r="AE288" s="11" t="n">
+        <v>40</v>
+      </c>
       <c r="AF288" s="11"/>
       <c r="AG288" s="11"/>
       <c r="AH288" s="11"/>
@@ -20927,7 +21154,9 @@
       <c r="AY288" s="11"/>
       <c r="AZ288" s="11"/>
       <c r="BA288" s="11"/>
-      <c r="BB288" s="11"/>
+      <c r="BB288" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="BC288" s="11"/>
       <c r="BD288" s="11"/>
       <c r="BE288" s="11"/>
@@ -20937,9 +21166,15 @@
       <c r="BI288" s="11"/>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="12"/>
-      <c r="B289" s="12"/>
-      <c r="C289" s="12"/>
+      <c r="A289" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B289" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C289" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D289" s="12"/>
       <c r="E289" s="12"/>
       <c r="F289" s="12"/>
@@ -20962,7 +21197,9 @@
       <c r="W289" s="12"/>
       <c r="X289" s="12"/>
       <c r="Y289" s="12"/>
-      <c r="Z289" s="12"/>
+      <c r="Z289" s="12" t="n">
+        <v>75</v>
+      </c>
       <c r="AA289" s="12"/>
       <c r="AB289" s="12"/>
       <c r="AC289" s="12"/>
@@ -21000,9 +21237,15 @@
       <c r="BI289" s="12"/>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="11"/>
-      <c r="B290" s="11"/>
-      <c r="C290" s="11"/>
+      <c r="A290" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B290" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C290" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D290" s="11"/>
       <c r="E290" s="11"/>
       <c r="F290" s="11"/>
@@ -21026,7 +21269,9 @@
       <c r="X290" s="11"/>
       <c r="Y290" s="11"/>
       <c r="Z290" s="11"/>
-      <c r="AA290" s="11"/>
+      <c r="AA290" s="11" t="n">
+        <v>75</v>
+      </c>
       <c r="AB290" s="11"/>
       <c r="AC290" s="11"/>
       <c r="AD290" s="11"/>
@@ -21063,9 +21308,15 @@
       <c r="BI290" s="11"/>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="12"/>
-      <c r="B291" s="12"/>
-      <c r="C291" s="12"/>
+      <c r="A291" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B291" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C291" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D291" s="12"/>
       <c r="E291" s="12"/>
       <c r="F291" s="12"/>
@@ -21089,7 +21340,9 @@
       <c r="X291" s="12"/>
       <c r="Y291" s="12"/>
       <c r="Z291" s="12"/>
-      <c r="AA291" s="12"/>
+      <c r="AA291" s="12" t="n">
+        <v>75</v>
+      </c>
       <c r="AB291" s="12"/>
       <c r="AC291" s="12"/>
       <c r="AD291" s="12"/>
@@ -21126,9 +21379,15 @@
       <c r="BI291" s="12"/>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="11"/>
-      <c r="B292" s="11"/>
-      <c r="C292" s="11"/>
+      <c r="A292" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B292" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C292" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D292" s="11"/>
       <c r="E292" s="11"/>
       <c r="F292" s="11"/>
@@ -21143,7 +21402,9 @@
       <c r="O292" s="11"/>
       <c r="P292" s="11"/>
       <c r="Q292" s="11"/>
-      <c r="R292" s="11"/>
+      <c r="R292" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="S292" s="11"/>
       <c r="T292" s="11"/>
       <c r="U292" s="11"/>
@@ -21189,9 +21450,15 @@
       <c r="BI292" s="11"/>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="12"/>
-      <c r="B293" s="12"/>
-      <c r="C293" s="12"/>
+      <c r="A293" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B293" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C293" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D293" s="12"/>
       <c r="E293" s="12"/>
       <c r="F293" s="12"/>
@@ -21217,7 +21484,9 @@
       <c r="Z293" s="12"/>
       <c r="AA293" s="12"/>
       <c r="AB293" s="12"/>
-      <c r="AC293" s="12"/>
+      <c r="AC293" s="12" t="n">
+        <v>40</v>
+      </c>
       <c r="AD293" s="12"/>
       <c r="AE293" s="12"/>
       <c r="AF293" s="12"/>
@@ -21252,9 +21521,15 @@
       <c r="BI293" s="12"/>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="11"/>
-      <c r="B294" s="11"/>
-      <c r="C294" s="11"/>
+      <c r="A294" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B294" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C294" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D294" s="11"/>
       <c r="E294" s="11"/>
       <c r="F294" s="11"/>
@@ -21275,7 +21550,9 @@
       <c r="U294" s="11"/>
       <c r="V294" s="11"/>
       <c r="W294" s="11"/>
-      <c r="X294" s="11"/>
+      <c r="X294" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="Y294" s="11"/>
       <c r="Z294" s="11"/>
       <c r="AA294" s="11"/>
@@ -21315,9 +21592,15 @@
       <c r="BI294" s="11"/>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="12"/>
-      <c r="B295" s="12"/>
-      <c r="C295" s="12"/>
+      <c r="A295" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B295" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C295" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D295" s="12"/>
       <c r="E295" s="12"/>
       <c r="F295" s="12"/>
@@ -21341,7 +21624,9 @@
       <c r="X295" s="12"/>
       <c r="Y295" s="12"/>
       <c r="Z295" s="12"/>
-      <c r="AA295" s="12"/>
+      <c r="AA295" s="12" t="n">
+        <v>75</v>
+      </c>
       <c r="AB295" s="12"/>
       <c r="AC295" s="12"/>
       <c r="AD295" s="12"/>
@@ -21378,9 +21663,15 @@
       <c r="BI295" s="12"/>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="11"/>
-      <c r="B296" s="11"/>
-      <c r="C296" s="11"/>
+      <c r="A296" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B296" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C296" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D296" s="11"/>
       <c r="E296" s="11"/>
       <c r="F296" s="11"/>
@@ -21401,7 +21692,9 @@
       <c r="U296" s="11"/>
       <c r="V296" s="11"/>
       <c r="W296" s="11"/>
-      <c r="X296" s="11"/>
+      <c r="X296" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="Y296" s="11"/>
       <c r="Z296" s="11"/>
       <c r="AA296" s="11"/>
@@ -21441,9 +21734,15 @@
       <c r="BI296" s="11"/>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="12"/>
-      <c r="B297" s="12"/>
-      <c r="C297" s="12"/>
+      <c r="A297" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B297" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C297" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D297" s="12"/>
       <c r="E297" s="12"/>
       <c r="F297" s="12"/>
@@ -21452,7 +21751,9 @@
       <c r="I297" s="12"/>
       <c r="J297" s="12"/>
       <c r="K297" s="12"/>
-      <c r="L297" s="12"/>
+      <c r="L297" s="12" t="n">
+        <v>20</v>
+      </c>
       <c r="M297" s="12"/>
       <c r="N297" s="12"/>
       <c r="O297" s="12"/>
@@ -21504,9 +21805,15 @@
       <c r="BI297" s="12"/>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="11"/>
-      <c r="B298" s="11"/>
-      <c r="C298" s="11"/>
+      <c r="A298" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B298" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C298" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D298" s="11"/>
       <c r="E298" s="11"/>
       <c r="F298" s="11"/>
@@ -21536,7 +21843,9 @@
       <c r="AD298" s="11"/>
       <c r="AE298" s="11"/>
       <c r="AF298" s="11"/>
-      <c r="AG298" s="11"/>
+      <c r="AG298" s="11" t="n">
+        <v>3000</v>
+      </c>
       <c r="AH298" s="11"/>
       <c r="AI298" s="11"/>
       <c r="AJ298" s="11"/>
@@ -21567,14 +21876,22 @@
       <c r="BI298" s="11"/>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="12"/>
-      <c r="B299" s="12"/>
-      <c r="C299" s="12"/>
+      <c r="A299" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B299" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C299" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D299" s="12"/>
       <c r="E299" s="12"/>
       <c r="F299" s="12"/>
       <c r="G299" s="12"/>
-      <c r="H299" s="12"/>
+      <c r="H299" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="I299" s="12"/>
       <c r="J299" s="12"/>
       <c r="K299" s="12"/>
@@ -21630,9 +21947,15 @@
       <c r="BI299" s="12"/>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="11"/>
-      <c r="B300" s="11"/>
-      <c r="C300" s="11"/>
+      <c r="A300" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B300" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C300" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D300" s="11"/>
       <c r="E300" s="11"/>
       <c r="F300" s="11"/>
@@ -21651,7 +21974,9 @@
       <c r="S300" s="11"/>
       <c r="T300" s="11"/>
       <c r="U300" s="11"/>
-      <c r="V300" s="11"/>
+      <c r="V300" s="11" t="n">
+        <v>50</v>
+      </c>
       <c r="W300" s="11"/>
       <c r="X300" s="11"/>
       <c r="Y300" s="11"/>
@@ -21683,7 +22008,9 @@
       <c r="AY300" s="11"/>
       <c r="AZ300" s="11"/>
       <c r="BA300" s="11"/>
-      <c r="BB300" s="11"/>
+      <c r="BB300" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="BC300" s="11"/>
       <c r="BD300" s="11"/>
       <c r="BE300" s="11"/>
@@ -21693,9 +22020,15 @@
       <c r="BI300" s="11"/>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="12"/>
-      <c r="B301" s="12"/>
-      <c r="C301" s="12"/>
+      <c r="A301" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B301" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C301" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="D301" s="12"/>
       <c r="E301" s="12"/>
       <c r="F301" s="12"/>
@@ -21714,7 +22047,9 @@
       <c r="S301" s="12"/>
       <c r="T301" s="12"/>
       <c r="U301" s="12"/>
-      <c r="V301" s="12"/>
+      <c r="V301" s="12" t="n">
+        <v>50</v>
+      </c>
       <c r="W301" s="12"/>
       <c r="X301" s="12"/>
       <c r="Y301" s="12"/>
@@ -21756,9 +22091,15 @@
       <c r="BI301" s="12"/>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="11"/>
-      <c r="B302" s="11"/>
-      <c r="C302" s="11"/>
+      <c r="A302" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B302" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C302" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="D302" s="11"/>
       <c r="E302" s="11"/>
       <c r="F302" s="11"/>
@@ -21788,7 +22129,9 @@
       <c r="AD302" s="11"/>
       <c r="AE302" s="11"/>
       <c r="AF302" s="11"/>
-      <c r="AG302" s="11"/>
+      <c r="AG302" s="11" t="n">
+        <v>370</v>
+      </c>
       <c r="AH302" s="11"/>
       <c r="AI302" s="11"/>
       <c r="AJ302" s="11"/>

</xml_diff>